<commit_message>
Update helper spreadsheets for 3.30.14
Small changes to be consistent with 3.30.14 input file standard comments.
</commit_message>
<xml_diff>
--- a/Helper_Spreadsheets/SS_330_starter_and_forecast_helper.xlsx
+++ b/Helper_Spreadsheets/SS_330_starter_and_forecast_helper.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Kathryn.Doering\Documents\Documents\vlab\helper_spreadsheet_update\Update_to_3.30.13\upload_to_vlab_June_2019\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Kathryn.Doering\Documents\Documents\vlab\helper_spreadsheet_update\update_to_3.30.14\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9600"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="11955" windowHeight="7485"/>
   </bookViews>
   <sheets>
     <sheet name="STARTER" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="105">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="105">
   <si>
     <t>#</t>
   </si>
@@ -172,9 +172,6 @@
     <t xml:space="preserve"> end_recruits</t>
   </si>
   <si>
-    <t>V3.30.13-safe;_2019_03_09;_Stock_Synthesis_by_Richard_Methot_(NOAA)_using_ADMB_12.0</t>
-  </si>
-  <si>
     <t>#Stock Synthesis (SS) is a work of the U.S. Government and is not subject to copyright protection in the United States.</t>
   </si>
   <si>
@@ -283,9 +280,6 @@
     <t># MCMC output detail: integer part (0=default; 1=adds obj func components); and decimal part (added to SR_LN(R0) on first call to mcmc)</t>
   </si>
   <si>
-    <t>#V3.30.13-safe;_2019_03_09;_Stock_Synthesis_by_Richard_Methot_(NOAA)_using_ADMB_12.0</t>
-  </si>
-  <si>
     <t xml:space="preserve"># verify end of input </t>
   </si>
   <si>
@@ -335,6 +329,12 @@
   </si>
   <si>
     <t># enter list of: fleet number, max annual catch for fleets with a max; terminate with fleet=-9999</t>
+  </si>
+  <si>
+    <t>#V3.30.14.00-safe;_2019_07_16;_Stock_Synthesis_by_Richard_Methot_(NOAA)_using_ADMB_12.0</t>
+  </si>
+  <si>
+    <t>3.30</t>
   </si>
 </sst>
 </file>
@@ -389,7 +389,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
@@ -399,6 +399,9 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1259,7 +1262,7 @@
   <dimension ref="A1:M36"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N39" sqref="N39"/>
+      <selection activeCell="E41" sqref="E41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1270,7 +1273,7 @@
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
-        <v>50</v>
+        <v>103</v>
       </c>
       <c r="B1" s="3"/>
       <c r="C1" s="3"/>
@@ -1287,7 +1290,7 @@
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B2" s="3"/>
       <c r="C2" s="3"/>
@@ -1304,7 +1307,7 @@
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B3" s="3"/>
       <c r="C3" s="3"/>
@@ -1321,7 +1324,7 @@
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B4" s="3"/>
       <c r="C4" s="3"/>
@@ -1338,7 +1341,7 @@
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B5" s="3"/>
       <c r="C5" s="3"/>
@@ -1355,10 +1358,10 @@
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C6" s="3"/>
       <c r="D6" s="3"/>
@@ -1374,10 +1377,10 @@
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C7" s="3"/>
       <c r="D7" s="3"/>
@@ -1396,7 +1399,7 @@
         <v>1</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C8" s="3"/>
       <c r="D8" s="3"/>
@@ -1415,7 +1418,7 @@
         <v>1</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C9" s="3"/>
       <c r="D9" s="3"/>
@@ -1434,7 +1437,7 @@
         <v>1</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C10" s="3"/>
       <c r="D10" s="3"/>
@@ -1453,7 +1456,7 @@
         <v>0</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C11" s="3"/>
       <c r="D11" s="3"/>
@@ -1472,7 +1475,7 @@
         <v>4</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C12" s="3"/>
       <c r="D12" s="3"/>
@@ -1491,7 +1494,7 @@
         <v>1</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C13" s="3"/>
       <c r="D13" s="3"/>
@@ -1510,7 +1513,7 @@
         <v>1</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C14" s="3"/>
       <c r="D14" s="3"/>
@@ -1529,7 +1532,7 @@
         <v>1</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C15" s="3"/>
       <c r="D15" s="3"/>
@@ -1548,7 +1551,7 @@
         <v>3</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C16" s="3"/>
       <c r="D16" s="3"/>
@@ -1567,7 +1570,7 @@
         <v>100</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C17" s="3"/>
       <c r="D17" s="3"/>
@@ -1586,7 +1589,7 @@
         <v>0</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C18" s="3"/>
       <c r="D18" s="3"/>
@@ -1605,7 +1608,7 @@
         <v>1</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C19" s="3"/>
       <c r="D19" s="3"/>
@@ -1624,7 +1627,7 @@
         <v>0</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C20" s="3"/>
       <c r="D20" s="3"/>
@@ -1643,7 +1646,7 @@
         <v>-1</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C21" s="3"/>
       <c r="D21" s="3"/>
@@ -1662,7 +1665,7 @@
         <v>-2</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C22" s="3"/>
       <c r="D22" s="3"/>
@@ -1681,7 +1684,7 @@
         <v>0</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C23" s="3"/>
       <c r="D23" s="3"/>
@@ -1717,7 +1720,7 @@
         <v>1E-4</v>
       </c>
       <c r="B25" s="3" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C25" s="3"/>
       <c r="D25" s="3"/>
@@ -1736,7 +1739,7 @@
         <v>0</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C26" s="3"/>
       <c r="D26" s="3"/>
@@ -1755,7 +1758,7 @@
         <v>1</v>
       </c>
       <c r="B27" s="3" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C27" s="3"/>
       <c r="D27" s="3"/>
@@ -1774,7 +1777,7 @@
         <v>2</v>
       </c>
       <c r="B28" s="3" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C28" s="3"/>
       <c r="D28" s="3"/>
@@ -1793,7 +1796,7 @@
         <v>1</v>
       </c>
       <c r="B29" s="3" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C29" s="3"/>
       <c r="D29" s="3"/>
@@ -1812,7 +1815,7 @@
         <v>4</v>
       </c>
       <c r="B30" s="3" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C30" s="3"/>
       <c r="D30" s="3"/>
@@ -1831,7 +1834,7 @@
         <v>3</v>
       </c>
       <c r="B31" s="3" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C31" s="3"/>
       <c r="D31" s="3"/>
@@ -1847,7 +1850,7 @@
     </row>
     <row r="32" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A32" s="3" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B32" s="3"/>
       <c r="C32" s="3"/>
@@ -1867,7 +1870,7 @@
         <v>0</v>
       </c>
       <c r="B33" s="3" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C33" s="3"/>
       <c r="D33" s="3"/>
@@ -1886,7 +1889,7 @@
         <v>0</v>
       </c>
       <c r="B34" s="3" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C34" s="3"/>
       <c r="D34" s="3"/>
@@ -1905,7 +1908,7 @@
         <v>0</v>
       </c>
       <c r="B35" s="3" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C35" s="3"/>
       <c r="D35" s="3"/>
@@ -1920,11 +1923,11 @@
       <c r="M35" s="3"/>
     </row>
     <row r="36" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A36" s="1">
-        <v>3.3</v>
+      <c r="A36" s="7" t="s">
+        <v>104</v>
       </c>
       <c r="B36" s="3" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C36" s="3"/>
       <c r="D36" s="3"/>
@@ -1940,6 +1943,9 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <ignoredErrors>
+    <ignoredError sqref="A36" numberStoredAsText="1"/>
+  </ignoredErrors>
 </worksheet>
 </file>
 
@@ -1947,9 +1953,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K64"/>
   <sheetViews>
-    <sheetView topLeftCell="A40" workbookViewId="0">
-      <selection activeCell="L27" sqref="L27"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1961,7 +1965,7 @@
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
-        <v>87</v>
+        <v>103</v>
       </c>
       <c r="B1" s="3"/>
       <c r="C1" s="3"/>
@@ -1976,7 +1980,7 @@
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B2" s="3"/>
       <c r="C2" s="3"/>
@@ -1991,7 +1995,7 @@
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B3" s="3"/>
       <c r="C3" s="3"/>
@@ -2321,7 +2325,7 @@
         <v>1</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="C20" s="3"/>
       <c r="D20" s="3"/>
@@ -2338,7 +2342,7 @@
         <v>1</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="C21" s="3"/>
       <c r="D21" s="3"/>
@@ -2355,7 +2359,7 @@
         <v>0</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="C22" s="3"/>
       <c r="D22" s="3"/>
@@ -2406,7 +2410,7 @@
         <v>0.75</v>
       </c>
       <c r="B25" s="3" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="C25" s="3"/>
       <c r="D25" s="3"/>
@@ -2423,7 +2427,7 @@
         <v>0</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="C26" s="3"/>
       <c r="D26" s="3"/>
@@ -2474,7 +2478,7 @@
         <v>1</v>
       </c>
       <c r="B29" s="3" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="C29" s="3"/>
       <c r="D29" s="3"/>
@@ -2491,7 +2495,7 @@
         <v>0</v>
       </c>
       <c r="B30" s="3" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="C30" s="3"/>
       <c r="D30" s="3"/>
@@ -2508,7 +2512,7 @@
         <v>1</v>
       </c>
       <c r="B31" s="3" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="C31" s="3"/>
       <c r="D31" s="3"/>
@@ -2703,7 +2707,7 @@
     </row>
     <row r="43" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A43" s="3" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="B43" s="3"/>
       <c r="C43" s="3"/>
@@ -2718,10 +2722,10 @@
     </row>
     <row r="44" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A44" s="3" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="B44" s="3" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="C44" s="3"/>
       <c r="D44" s="3"/>
@@ -2735,10 +2739,10 @@
     </row>
     <row r="45" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A45" s="3" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="B45" s="3" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="C45" s="3"/>
       <c r="D45" s="3"/>
@@ -2752,10 +2756,10 @@
     </row>
     <row r="46" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A46" s="3" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="B46" s="3" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="C46" s="3"/>
       <c r="D46" s="3"/>
@@ -2769,7 +2773,7 @@
     </row>
     <row r="47" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A47" s="3" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="B47" s="3"/>
       <c r="C47" s="3"/>
@@ -3049,7 +3053,7 @@
         <v>999</v>
       </c>
       <c r="B64" s="3" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="C64" s="3"/>
       <c r="D64" s="3"/>

</xml_diff>

<commit_message>
#66582 update description of no_forecast for 3.30.15
</commit_message>
<xml_diff>
--- a/Helper_Spreadsheets/SS_330_starter_and_forecast_helper.xlsx
+++ b/Helper_Spreadsheets/SS_330_starter_and_forecast_helper.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Kathryn.Doering\Documents\Documents\vlab\helper_spreadsheet_update\update_to_3.30.14\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Kathryn.Doering\Documents\Documents\Stock_Synthesis\vlab_repo\SS_documentation\ss_documentation\Helper_Spreadsheets\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="11955" windowHeight="7485"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="11955" windowHeight="7485" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="STARTER" sheetId="1" r:id="rId1"/>
@@ -91,9 +91,6 @@
     <t>#_Bmark_years:   enter actual year, or -999 for styr, or value &lt;=0 to be relative to endyr</t>
   </si>
   <si>
-    <t># Forecast: 0=none; 1=F(SPR); 2=F(MSY) 3=F(Btgt); 4=Ave F (uses first-last relF yrs); 5=input annual F scalar</t>
-  </si>
-  <si>
     <t xml:space="preserve"># N forecast years </t>
   </si>
   <si>
@@ -335,6 +332,9 @@
   </si>
   <si>
     <t>3.30</t>
+  </si>
+  <si>
+    <t># Forecast:  -1=none; 0=simple; 1=F(SPR); 2=F(MSY) 3=F(Btgt) or F0.1; 4=Ave F (uses first-last relF yrs); 5=input annual F scalar</t>
   </si>
 </sst>
 </file>
@@ -521,15 +521,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>11</xdr:col>
-      <xdr:colOff>85725</xdr:colOff>
-      <xdr:row>10</xdr:row>
-      <xdr:rowOff>47625</xdr:rowOff>
+      <xdr:colOff>285750</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>142875</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>18</xdr:col>
-      <xdr:colOff>180975</xdr:colOff>
+      <xdr:colOff>381000</xdr:colOff>
       <xdr:row>19</xdr:row>
-      <xdr:rowOff>152400</xdr:rowOff>
+      <xdr:rowOff>57150</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -538,7 +538,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="7953375" y="1952625"/>
+          <a:off x="8153400" y="1857375"/>
           <a:ext cx="4362450" cy="1819275"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -969,6 +969,175 @@
     </xdr:cxnSp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>485775</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>104774</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>581025</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>47625</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="9" name="TextBox 8"/>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="8353425" y="4105274"/>
+          <a:ext cx="4362450" cy="1657351"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFF00"/>
+        </a:solidFill>
+        <a:ln w="9525" cmpd="sng">
+          <a:solidFill>
+            <a:schemeClr val="lt1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1600" b="1"/>
+            <a:t>Forecast type options</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>- 1 is an option as of 3.30.15. Use this if no forecast is required</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>0 is a simple forecast of 1 year</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="en-US" sz="1100" b="0" baseline="0">
+            <a:solidFill>
+              <a:schemeClr val="dk1"/>
+            </a:solidFill>
+            <a:effectLst/>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>If -1 or 0 is used, then no input is required after the FORECAST type specification (if there is any, SS will ignore all remaining values in the file.</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="en-US">
+            <a:effectLst/>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>438151</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>447675</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>161925</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="11" name="Straight Arrow Connector 10"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1" flipV="1">
+          <a:off x="1866901" y="2476500"/>
+          <a:ext cx="6448424" cy="1685925"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="arrow"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -1261,7 +1430,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M36"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E41" sqref="E41"/>
     </sheetView>
   </sheetViews>
@@ -1273,7 +1442,7 @@
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B1" s="3"/>
       <c r="C1" s="3"/>
@@ -1290,7 +1459,7 @@
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B2" s="3"/>
       <c r="C2" s="3"/>
@@ -1307,7 +1476,7 @@
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B3" s="3"/>
       <c r="C3" s="3"/>
@@ -1324,7 +1493,7 @@
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B4" s="3"/>
       <c r="C4" s="3"/>
@@ -1341,7 +1510,7 @@
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B5" s="3"/>
       <c r="C5" s="3"/>
@@ -1358,10 +1527,10 @@
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C6" s="3"/>
       <c r="D6" s="3"/>
@@ -1377,10 +1546,10 @@
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C7" s="3"/>
       <c r="D7" s="3"/>
@@ -1399,7 +1568,7 @@
         <v>1</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C8" s="3"/>
       <c r="D8" s="3"/>
@@ -1418,7 +1587,7 @@
         <v>1</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C9" s="3"/>
       <c r="D9" s="3"/>
@@ -1437,7 +1606,7 @@
         <v>1</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C10" s="3"/>
       <c r="D10" s="3"/>
@@ -1456,7 +1625,7 @@
         <v>0</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C11" s="3"/>
       <c r="D11" s="3"/>
@@ -1475,7 +1644,7 @@
         <v>4</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C12" s="3"/>
       <c r="D12" s="3"/>
@@ -1494,7 +1663,7 @@
         <v>1</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C13" s="3"/>
       <c r="D13" s="3"/>
@@ -1513,7 +1682,7 @@
         <v>1</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C14" s="3"/>
       <c r="D14" s="3"/>
@@ -1532,7 +1701,7 @@
         <v>1</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C15" s="3"/>
       <c r="D15" s="3"/>
@@ -1551,7 +1720,7 @@
         <v>3</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C16" s="3"/>
       <c r="D16" s="3"/>
@@ -1570,7 +1739,7 @@
         <v>100</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C17" s="3"/>
       <c r="D17" s="3"/>
@@ -1589,7 +1758,7 @@
         <v>0</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C18" s="3"/>
       <c r="D18" s="3"/>
@@ -1608,7 +1777,7 @@
         <v>1</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C19" s="3"/>
       <c r="D19" s="3"/>
@@ -1627,7 +1796,7 @@
         <v>0</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C20" s="3"/>
       <c r="D20" s="3"/>
@@ -1646,7 +1815,7 @@
         <v>-1</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C21" s="3"/>
       <c r="D21" s="3"/>
@@ -1665,7 +1834,7 @@
         <v>-2</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C22" s="3"/>
       <c r="D22" s="3"/>
@@ -1684,7 +1853,7 @@
         <v>0</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C23" s="3"/>
       <c r="D23" s="3"/>
@@ -1700,7 +1869,7 @@
     </row>
     <row r="24" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A24" s="3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B24" s="3"/>
       <c r="C24" s="3"/>
@@ -1720,7 +1889,7 @@
         <v>1E-4</v>
       </c>
       <c r="B25" s="3" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C25" s="3"/>
       <c r="D25" s="3"/>
@@ -1739,7 +1908,7 @@
         <v>0</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C26" s="3"/>
       <c r="D26" s="3"/>
@@ -1758,7 +1927,7 @@
         <v>1</v>
       </c>
       <c r="B27" s="3" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C27" s="3"/>
       <c r="D27" s="3"/>
@@ -1777,7 +1946,7 @@
         <v>2</v>
       </c>
       <c r="B28" s="3" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C28" s="3"/>
       <c r="D28" s="3"/>
@@ -1796,7 +1965,7 @@
         <v>1</v>
       </c>
       <c r="B29" s="3" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C29" s="3"/>
       <c r="D29" s="3"/>
@@ -1815,7 +1984,7 @@
         <v>4</v>
       </c>
       <c r="B30" s="3" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C30" s="3"/>
       <c r="D30" s="3"/>
@@ -1834,7 +2003,7 @@
         <v>3</v>
       </c>
       <c r="B31" s="3" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C31" s="3"/>
       <c r="D31" s="3"/>
@@ -1850,7 +2019,7 @@
     </row>
     <row r="32" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A32" s="3" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B32" s="3"/>
       <c r="C32" s="3"/>
@@ -1870,7 +2039,7 @@
         <v>0</v>
       </c>
       <c r="B33" s="3" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C33" s="3"/>
       <c r="D33" s="3"/>
@@ -1889,7 +2058,7 @@
         <v>0</v>
       </c>
       <c r="B34" s="3" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C34" s="3"/>
       <c r="D34" s="3"/>
@@ -1908,7 +2077,7 @@
         <v>0</v>
       </c>
       <c r="B35" s="3" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C35" s="3"/>
       <c r="D35" s="3"/>
@@ -1924,10 +2093,10 @@
     </row>
     <row r="36" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A36" s="7" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B36" s="3" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C36" s="3"/>
       <c r="D36" s="3"/>
@@ -1953,7 +2122,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K64"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="V15" sqref="V15"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1965,7 +2136,7 @@
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B1" s="3"/>
       <c r="C1" s="3"/>
@@ -1980,7 +2151,7 @@
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B2" s="3"/>
       <c r="C2" s="3"/>
@@ -1995,7 +2166,7 @@
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B3" s="3"/>
       <c r="C3" s="3"/>
@@ -2111,16 +2282,16 @@
         <v>21</v>
       </c>
       <c r="G9" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="H9" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="H9" s="3" t="s">
+      <c r="I9" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="I9" s="3" t="s">
+      <c r="J9" s="3" t="s">
         <v>46</v>
-      </c>
-      <c r="J9" s="3" t="s">
-        <v>47</v>
       </c>
       <c r="K9" s="6"/>
     </row>
@@ -2194,7 +2365,7 @@
         <v>1</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>23</v>
+        <v>104</v>
       </c>
       <c r="C13" s="3"/>
       <c r="D13" s="3"/>
@@ -2211,7 +2382,7 @@
         <v>2</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C14" s="3"/>
       <c r="D14" s="3"/>
@@ -2228,7 +2399,7 @@
         <v>0.2</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C15" s="3"/>
       <c r="D15" s="3"/>
@@ -2242,7 +2413,7 @@
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B16" s="3"/>
       <c r="C16" s="3"/>
@@ -2257,7 +2428,7 @@
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B17" s="3" t="s">
         <v>19</v>
@@ -2269,10 +2440,10 @@
         <v>21</v>
       </c>
       <c r="E17" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="F17" s="3" t="s">
         <v>48</v>
-      </c>
-      <c r="F17" s="3" t="s">
-        <v>49</v>
       </c>
       <c r="G17" s="3"/>
       <c r="H17" s="3"/>
@@ -2325,7 +2496,7 @@
         <v>1</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C20" s="3"/>
       <c r="D20" s="3"/>
@@ -2342,7 +2513,7 @@
         <v>1</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C21" s="3"/>
       <c r="D21" s="3"/>
@@ -2359,7 +2530,7 @@
         <v>0</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C22" s="3"/>
       <c r="D22" s="3"/>
@@ -2376,7 +2547,7 @@
         <v>0.4</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C23" s="3"/>
       <c r="D23" s="3"/>
@@ -2393,7 +2564,7 @@
         <v>0.1</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C24" s="3"/>
       <c r="D24" s="3"/>
@@ -2410,7 +2581,7 @@
         <v>0.75</v>
       </c>
       <c r="B25" s="3" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C25" s="3"/>
       <c r="D25" s="3"/>
@@ -2427,7 +2598,7 @@
         <v>0</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C26" s="3"/>
       <c r="D26" s="3"/>
@@ -2444,7 +2615,7 @@
         <v>3</v>
       </c>
       <c r="B27" s="3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C27" s="3"/>
       <c r="D27" s="3"/>
@@ -2461,7 +2632,7 @@
         <v>3</v>
       </c>
       <c r="B28" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C28" s="3"/>
       <c r="D28" s="3"/>
@@ -2478,7 +2649,7 @@
         <v>1</v>
       </c>
       <c r="B29" s="3" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C29" s="3"/>
       <c r="D29" s="3"/>
@@ -2495,7 +2666,7 @@
         <v>0</v>
       </c>
       <c r="B30" s="3" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C30" s="3"/>
       <c r="D30" s="3"/>
@@ -2512,7 +2683,7 @@
         <v>1</v>
       </c>
       <c r="B31" s="3" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C31" s="3"/>
       <c r="D31" s="3"/>
@@ -2529,7 +2700,7 @@
         <v>0</v>
       </c>
       <c r="B32" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C32" s="3"/>
       <c r="D32" s="3"/>
@@ -2561,7 +2732,7 @@
         <v>2010</v>
       </c>
       <c r="B34" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C34" s="3"/>
       <c r="D34" s="3"/>
@@ -2578,7 +2749,7 @@
         <v>0</v>
       </c>
       <c r="B35" s="3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C35" s="3"/>
       <c r="D35" s="3"/>
@@ -2595,7 +2766,7 @@
         <v>0</v>
       </c>
       <c r="B36" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C36" s="3"/>
       <c r="D36" s="3"/>
@@ -2612,7 +2783,7 @@
         <v>1999</v>
       </c>
       <c r="B37" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C37" s="3"/>
       <c r="D37" s="3"/>
@@ -2629,7 +2800,7 @@
         <v>2002</v>
       </c>
       <c r="B38" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C38" s="3"/>
       <c r="D38" s="3"/>
@@ -2707,7 +2878,7 @@
     </row>
     <row r="43" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A43" s="3" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B43" s="3"/>
       <c r="C43" s="3"/>
@@ -2722,10 +2893,10 @@
     </row>
     <row r="44" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A44" s="3" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B44" s="3" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C44" s="3"/>
       <c r="D44" s="3"/>
@@ -2739,10 +2910,10 @@
     </row>
     <row r="45" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A45" s="3" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B45" s="3" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C45" s="3"/>
       <c r="D45" s="3"/>
@@ -2756,10 +2927,10 @@
     </row>
     <row r="46" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A46" s="3" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B46" s="3" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C46" s="3"/>
       <c r="D46" s="3"/>
@@ -2773,7 +2944,7 @@
     </row>
     <row r="47" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A47" s="3" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B47" s="3"/>
       <c r="C47" s="3"/>
@@ -2805,7 +2976,7 @@
     </row>
     <row r="49" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A49" s="3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B49" s="3"/>
       <c r="C49" s="3"/>
@@ -2837,7 +3008,7 @@
     </row>
     <row r="51" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A51" s="3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B51" s="3"/>
       <c r="C51" s="3"/>
@@ -2869,7 +3040,7 @@
     </row>
     <row r="53" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A53" s="3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B53" s="3"/>
       <c r="C53" s="3"/>
@@ -2946,7 +3117,7 @@
     </row>
     <row r="58" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A58" s="3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B58" s="3"/>
       <c r="C58" s="3"/>
@@ -2993,7 +3164,7 @@
     </row>
     <row r="61" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A61" s="3" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B61" s="3" t="s">
         <v>13</v>
@@ -3002,7 +3173,7 @@
         <v>14</v>
       </c>
       <c r="D61" s="3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E61" s="3"/>
       <c r="F61" s="3"/>
@@ -3053,7 +3224,7 @@
         <v>999</v>
       </c>
       <c r="B64" s="3" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C64" s="3"/>
       <c r="D64" s="3"/>

</xml_diff>

<commit_message>
#72993 and #67971 : document random seed feature in helper spreadsheets
</commit_message>
<xml_diff>
--- a/Helper_Spreadsheets/SS_330_starter_and_forecast_helper.xlsx
+++ b/Helper_Spreadsheets/SS_330_starter_and_forecast_helper.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="11955" windowHeight="7485" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="11955" windowHeight="7485"/>
   </bookViews>
   <sheets>
     <sheet name="STARTER" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="105">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="107">
   <si>
     <t>#</t>
   </si>
@@ -335,13 +335,42 @@
   </si>
   <si>
     <t># Forecast:  -1=none; 0=simple; 1=F(SPR); 2=F(MSY) 3=F(Btgt) or F0.1; 4=Ave F (uses first-last relF yrs); 5=input annual F scalar</t>
+  </si>
+  <si>
+    <t># set seed value</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">An </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>optional</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> line. If you do not wish to specify a seed, skip this line and end the reading of the file with the check value.</t>
+    </r>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -356,8 +385,16 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -376,8 +413,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -385,11 +428,48 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
@@ -402,6 +482,9 @@
     <xf numFmtId="49" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1428,10 +1511,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M36"/>
+  <dimension ref="A1:N37"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E41" sqref="E41"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G20" sqref="G20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1440,7 +1523,7 @@
     <col min="6" max="12" width="10.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>102</v>
       </c>
@@ -1456,8 +1539,9 @@
       <c r="K1" s="3"/>
       <c r="L1" s="3"/>
       <c r="M1" s="3"/>
-    </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N1" s="3"/>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>49</v>
       </c>
@@ -1473,8 +1557,9 @@
       <c r="K2" s="3"/>
       <c r="L2" s="3"/>
       <c r="M2" s="3"/>
-    </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N2" s="3"/>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>50</v>
       </c>
@@ -1490,8 +1575,9 @@
       <c r="K3" s="3"/>
       <c r="L3" s="3"/>
       <c r="M3" s="3"/>
-    </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N3" s="3"/>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>51</v>
       </c>
@@ -1507,8 +1593,9 @@
       <c r="K4" s="3"/>
       <c r="L4" s="3"/>
       <c r="M4" s="3"/>
-    </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N4" s="3"/>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>52</v>
       </c>
@@ -1524,8 +1611,9 @@
       <c r="K5" s="3"/>
       <c r="L5" s="3"/>
       <c r="M5" s="3"/>
-    </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N5" s="3"/>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>55</v>
       </c>
@@ -1543,8 +1631,9 @@
       <c r="K6" s="3"/>
       <c r="L6" s="3"/>
       <c r="M6" s="3"/>
-    </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N6" s="3"/>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>56</v>
       </c>
@@ -1562,8 +1651,9 @@
       <c r="K7" s="3"/>
       <c r="L7" s="3"/>
       <c r="M7" s="3"/>
-    </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N7" s="3"/>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A8" s="2">
         <v>1</v>
       </c>
@@ -1581,8 +1671,9 @@
       <c r="K8" s="3"/>
       <c r="L8" s="3"/>
       <c r="M8" s="3"/>
-    </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N8" s="3"/>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A9" s="2">
         <v>1</v>
       </c>
@@ -1600,8 +1691,9 @@
       <c r="K9" s="3"/>
       <c r="L9" s="3"/>
       <c r="M9" s="3"/>
-    </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N9" s="3"/>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>1</v>
       </c>
@@ -1619,8 +1711,9 @@
       <c r="K10" s="3"/>
       <c r="L10" s="3"/>
       <c r="M10" s="3"/>
-    </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N10" s="3"/>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>0</v>
       </c>
@@ -1638,8 +1731,9 @@
       <c r="K11" s="3"/>
       <c r="L11" s="3"/>
       <c r="M11" s="3"/>
-    </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N11" s="3"/>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>4</v>
       </c>
@@ -1657,8 +1751,9 @@
       <c r="K12" s="3"/>
       <c r="L12" s="3"/>
       <c r="M12" s="3"/>
-    </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N12" s="3"/>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>1</v>
       </c>
@@ -1676,8 +1771,9 @@
       <c r="K13" s="3"/>
       <c r="L13" s="3"/>
       <c r="M13" s="3"/>
-    </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N13" s="3"/>
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <v>1</v>
       </c>
@@ -1695,8 +1791,9 @@
       <c r="K14" s="3"/>
       <c r="L14" s="3"/>
       <c r="M14" s="3"/>
-    </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N14" s="3"/>
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
         <v>1</v>
       </c>
@@ -1714,8 +1811,9 @@
       <c r="K15" s="3"/>
       <c r="L15" s="3"/>
       <c r="M15" s="3"/>
-    </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N15" s="3"/>
+    </row>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
         <v>3</v>
       </c>
@@ -1733,8 +1831,9 @@
       <c r="K16" s="3"/>
       <c r="L16" s="3"/>
       <c r="M16" s="3"/>
-    </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N16" s="3"/>
+    </row>
+    <row r="17" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
         <v>100</v>
       </c>
@@ -1752,8 +1851,9 @@
       <c r="K17" s="3"/>
       <c r="L17" s="3"/>
       <c r="M17" s="3"/>
-    </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N17" s="3"/>
+    </row>
+    <row r="18" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
         <v>0</v>
       </c>
@@ -1771,8 +1871,9 @@
       <c r="K18" s="3"/>
       <c r="L18" s="3"/>
       <c r="M18" s="3"/>
-    </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N18" s="3"/>
+    </row>
+    <row r="19" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
         <v>1</v>
       </c>
@@ -1790,8 +1891,9 @@
       <c r="K19" s="3"/>
       <c r="L19" s="3"/>
       <c r="M19" s="3"/>
-    </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N19" s="3"/>
+    </row>
+    <row r="20" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
         <v>0</v>
       </c>
@@ -1809,8 +1911,9 @@
       <c r="K20" s="3"/>
       <c r="L20" s="3"/>
       <c r="M20" s="3"/>
-    </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N20" s="3"/>
+    </row>
+    <row r="21" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
         <v>-1</v>
       </c>
@@ -1828,8 +1931,9 @@
       <c r="K21" s="3"/>
       <c r="L21" s="3"/>
       <c r="M21" s="3"/>
-    </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N21" s="3"/>
+    </row>
+    <row r="22" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
         <v>-2</v>
       </c>
@@ -1847,8 +1951,9 @@
       <c r="K22" s="3"/>
       <c r="L22" s="3"/>
       <c r="M22" s="3"/>
-    </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N22" s="3"/>
+    </row>
+    <row r="23" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A23" s="1">
         <v>0</v>
       </c>
@@ -1866,8 +1971,9 @@
       <c r="K23" s="3"/>
       <c r="L23" s="3"/>
       <c r="M23" s="3"/>
-    </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N23" s="3"/>
+    </row>
+    <row r="24" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A24" s="3" t="s">
         <v>37</v>
       </c>
@@ -1883,8 +1989,9 @@
       <c r="K24" s="3"/>
       <c r="L24" s="3"/>
       <c r="M24" s="3"/>
-    </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N24" s="3"/>
+    </row>
+    <row r="25" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A25" s="1">
         <v>1E-4</v>
       </c>
@@ -1902,8 +2009,9 @@
       <c r="K25" s="3"/>
       <c r="L25" s="3"/>
       <c r="M25" s="3"/>
-    </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N25" s="3"/>
+    </row>
+    <row r="26" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A26" s="1">
         <v>0</v>
       </c>
@@ -1921,8 +2029,9 @@
       <c r="K26" s="3"/>
       <c r="L26" s="3"/>
       <c r="M26" s="3"/>
-    </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N26" s="3"/>
+    </row>
+    <row r="27" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A27" s="1">
         <v>1</v>
       </c>
@@ -1940,8 +2049,9 @@
       <c r="K27" s="3"/>
       <c r="L27" s="3"/>
       <c r="M27" s="3"/>
-    </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N27" s="3"/>
+    </row>
+    <row r="28" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A28" s="1">
         <v>2</v>
       </c>
@@ -1959,8 +2069,9 @@
       <c r="K28" s="3"/>
       <c r="L28" s="3"/>
       <c r="M28" s="3"/>
-    </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N28" s="3"/>
+    </row>
+    <row r="29" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A29" s="1">
         <v>1</v>
       </c>
@@ -1978,8 +2089,9 @@
       <c r="K29" s="3"/>
       <c r="L29" s="3"/>
       <c r="M29" s="3"/>
-    </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N29" s="3"/>
+    </row>
+    <row r="30" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A30" s="1">
         <v>4</v>
       </c>
@@ -1997,8 +2109,9 @@
       <c r="K30" s="3"/>
       <c r="L30" s="3"/>
       <c r="M30" s="3"/>
-    </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N30" s="3"/>
+    </row>
+    <row r="31" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A31" s="1">
         <v>3</v>
       </c>
@@ -2016,8 +2129,9 @@
       <c r="K31" s="3"/>
       <c r="L31" s="3"/>
       <c r="M31" s="3"/>
-    </row>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N31" s="3"/>
+    </row>
+    <row r="32" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A32" s="3" t="s">
         <v>83</v>
       </c>
@@ -2033,8 +2147,9 @@
       <c r="K32" s="3"/>
       <c r="L32" s="3"/>
       <c r="M32" s="3"/>
-    </row>
-    <row r="33" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N32" s="3"/>
+    </row>
+    <row r="33" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A33" s="1">
         <v>0</v>
       </c>
@@ -2052,8 +2167,9 @@
       <c r="K33" s="3"/>
       <c r="L33" s="3"/>
       <c r="M33" s="3"/>
-    </row>
-    <row r="34" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N33" s="3"/>
+    </row>
+    <row r="34" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A34" s="1">
         <v>0</v>
       </c>
@@ -2071,8 +2187,9 @@
       <c r="K34" s="3"/>
       <c r="L34" s="3"/>
       <c r="M34" s="3"/>
-    </row>
-    <row r="35" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N34" s="3"/>
+    </row>
+    <row r="35" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A35" s="1">
         <v>0</v>
       </c>
@@ -2090,30 +2207,54 @@
       <c r="K35" s="3"/>
       <c r="L35" s="3"/>
       <c r="M35" s="3"/>
-    </row>
-    <row r="36" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A36" s="7" t="s">
+      <c r="N35" s="3"/>
+    </row>
+    <row r="36" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A36" s="1">
+        <v>123</v>
+      </c>
+      <c r="B36" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="C36" s="3"/>
+      <c r="D36" s="8" t="s">
+        <v>106</v>
+      </c>
+      <c r="E36" s="9"/>
+      <c r="F36" s="9"/>
+      <c r="G36" s="9"/>
+      <c r="H36" s="9"/>
+      <c r="I36" s="9"/>
+      <c r="J36" s="9"/>
+      <c r="K36" s="9"/>
+      <c r="L36" s="9"/>
+      <c r="M36" s="9"/>
+      <c r="N36" s="10"/>
+    </row>
+    <row r="37" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A37" s="7" t="s">
         <v>103</v>
       </c>
-      <c r="B36" s="3" t="s">
+      <c r="B37" s="3" t="s">
         <v>73</v>
       </c>
-      <c r="C36" s="3"/>
-      <c r="D36" s="3"/>
-      <c r="E36" s="3"/>
-      <c r="F36" s="3"/>
-      <c r="G36" s="3"/>
-      <c r="H36" s="3"/>
-      <c r="I36" s="3"/>
-      <c r="J36" s="3"/>
-      <c r="K36" s="3"/>
-      <c r="L36" s="3"/>
-      <c r="M36" s="3"/>
+      <c r="C37" s="3"/>
+      <c r="D37" s="3"/>
+      <c r="E37" s="3"/>
+      <c r="F37" s="3"/>
+      <c r="G37" s="3"/>
+      <c r="H37" s="3"/>
+      <c r="I37" s="3"/>
+      <c r="J37" s="3"/>
+      <c r="K37" s="3"/>
+      <c r="L37" s="3"/>
+      <c r="M37" s="3"/>
+      <c r="N37" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <ignoredErrors>
-    <ignoredError sqref="A36" numberStoredAsText="1"/>
+    <ignoredError sqref="A37" numberStoredAsText="1"/>
   </ignoredErrors>
 </worksheet>
 </file>
@@ -2122,8 +2263,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K64"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="V15" sqref="V15"/>
+    <sheetView topLeftCell="A43" workbookViewId="0">
+      <selection activeCell="C70" sqref="C70"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
#46175: describe starter input for custom reporting
</commit_message>
<xml_diff>
--- a/Helper_Spreadsheets/SS_330_starter_and_forecast_helper.xlsx
+++ b/Helper_Spreadsheets/SS_330_starter_and_forecast_helper.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="107">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="112">
   <si>
     <t>#</t>
   </si>
@@ -191,9 +191,6 @@
   </si>
   <si>
     <t>simple.ctl</t>
-  </si>
-  <si>
-    <t xml:space="preserve"># detailed output (0=minimal for data-limited, 1=high (w/ wtatage.ss_new), 2=brief) </t>
   </si>
   <si>
     <t># 0=use init values in control file; 1=use ss.par</t>
@@ -364,6 +361,24 @@
       </rPr>
       <t xml:space="preserve"> line. If you do not wish to specify a seed, skip this line and end the reading of the file with the check value.</t>
     </r>
+  </si>
+  <si>
+    <t xml:space="preserve"># detailed output (0=minimal for data-limited, 1=high (w/ wtatage.ss_new), 2=brief, 3=custom) </t>
+  </si>
+  <si>
+    <t># custom report options: -100 to start with minimal; -101 to start with all; -number to remove, +number to add, -999 to end</t>
+  </si>
+  <si>
+    <t># COND -100 # use -100 to start with minimal, or - 101 to start with all</t>
+  </si>
+  <si>
+    <t># COND -999  # terminator line</t>
+  </si>
+  <si>
+    <t xml:space="preserve"># COND 8  9  # Negative numbers for items to remove, Positive numbers for items to add. </t>
+  </si>
+  <si>
+    <t># Following COND lines only if detailed output = 3:</t>
   </si>
 </sst>
 </file>
@@ -1511,11 +1526,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N37"/>
+  <dimension ref="A1:N42"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G20" sqref="G20"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1525,7 +1538,7 @@
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B1" s="3"/>
       <c r="C1" s="3"/>
@@ -1658,7 +1671,7 @@
         <v>1</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C8" s="3"/>
       <c r="D8" s="3"/>
@@ -1678,7 +1691,7 @@
         <v>1</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C9" s="3"/>
       <c r="D9" s="3"/>
@@ -1698,7 +1711,7 @@
         <v>1</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>57</v>
+        <v>106</v>
       </c>
       <c r="C10" s="3"/>
       <c r="D10" s="3"/>
@@ -1714,19 +1727,17 @@
       <c r="N10" s="3"/>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A11" s="1">
-        <v>0</v>
-      </c>
-      <c r="B11" s="3" t="s">
-        <v>60</v>
-      </c>
+      <c r="A11" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="B11" s="3"/>
       <c r="C11" s="3"/>
       <c r="D11" s="3"/>
       <c r="E11" s="3"/>
       <c r="F11" s="3"/>
-      <c r="G11" s="3"/>
-      <c r="H11" s="3"/>
-      <c r="I11" s="3"/>
+      <c r="G11" s="4"/>
+      <c r="H11" s="4"/>
+      <c r="I11" s="4"/>
       <c r="J11" s="3"/>
       <c r="K11" s="3"/>
       <c r="L11" s="3"/>
@@ -1734,19 +1745,17 @@
       <c r="N11" s="3"/>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A12" s="1">
-        <v>4</v>
-      </c>
-      <c r="B12" s="3" t="s">
-        <v>61</v>
-      </c>
+      <c r="A12" s="3" t="s">
+        <v>107</v>
+      </c>
+      <c r="B12" s="3"/>
       <c r="C12" s="3"/>
       <c r="D12" s="3"/>
       <c r="E12" s="3"/>
       <c r="F12" s="3"/>
-      <c r="G12" s="3"/>
-      <c r="H12" s="3"/>
-      <c r="I12" s="3"/>
+      <c r="G12" s="4"/>
+      <c r="H12" s="4"/>
+      <c r="I12" s="4"/>
       <c r="J12" s="3"/>
       <c r="K12" s="3"/>
       <c r="L12" s="3"/>
@@ -1754,19 +1763,17 @@
       <c r="N12" s="3"/>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A13" s="1">
-        <v>1</v>
-      </c>
-      <c r="B13" s="3" t="s">
-        <v>62</v>
-      </c>
+      <c r="A13" s="3" t="s">
+        <v>108</v>
+      </c>
+      <c r="B13" s="3"/>
       <c r="C13" s="3"/>
       <c r="D13" s="3"/>
       <c r="E13" s="3"/>
       <c r="F13" s="3"/>
-      <c r="G13" s="3"/>
-      <c r="H13" s="3"/>
-      <c r="I13" s="3"/>
+      <c r="G13" s="4"/>
+      <c r="H13" s="4"/>
+      <c r="I13" s="4"/>
       <c r="J13" s="3"/>
       <c r="K13" s="3"/>
       <c r="L13" s="3"/>
@@ -1774,19 +1781,17 @@
       <c r="N13" s="3"/>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A14" s="1">
-        <v>1</v>
-      </c>
-      <c r="B14" s="3" t="s">
-        <v>63</v>
-      </c>
+      <c r="A14" s="3" t="s">
+        <v>110</v>
+      </c>
+      <c r="B14" s="3"/>
       <c r="C14" s="3"/>
       <c r="D14" s="3"/>
       <c r="E14" s="3"/>
       <c r="F14" s="3"/>
-      <c r="G14" s="3"/>
-      <c r="H14" s="3"/>
-      <c r="I14" s="3"/>
+      <c r="G14" s="4"/>
+      <c r="H14" s="4"/>
+      <c r="I14" s="4"/>
       <c r="J14" s="3"/>
       <c r="K14" s="3"/>
       <c r="L14" s="3"/>
@@ -1794,19 +1799,17 @@
       <c r="N14" s="3"/>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A15" s="1">
-        <v>1</v>
-      </c>
-      <c r="B15" s="3" t="s">
-        <v>64</v>
-      </c>
+      <c r="A15" s="3" t="s">
+        <v>109</v>
+      </c>
+      <c r="B15" s="3"/>
       <c r="C15" s="3"/>
       <c r="D15" s="3"/>
       <c r="E15" s="3"/>
       <c r="F15" s="3"/>
-      <c r="G15" s="3"/>
-      <c r="H15" s="3"/>
-      <c r="I15" s="3"/>
+      <c r="G15" s="4"/>
+      <c r="H15" s="4"/>
+      <c r="I15" s="4"/>
       <c r="J15" s="3"/>
       <c r="K15" s="3"/>
       <c r="L15" s="3"/>
@@ -1815,10 +1818,10 @@
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
       <c r="C16" s="3"/>
       <c r="D16" s="3"/>
@@ -1835,10 +1838,10 @@
     </row>
     <row r="17" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
-        <v>100</v>
+        <v>4</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
       <c r="C17" s="3"/>
       <c r="D17" s="3"/>
@@ -1855,10 +1858,10 @@
     </row>
     <row r="18" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>67</v>
+        <v>61</v>
       </c>
       <c r="C18" s="3"/>
       <c r="D18" s="3"/>
@@ -1878,7 +1881,7 @@
         <v>1</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>68</v>
+        <v>62</v>
       </c>
       <c r="C19" s="3"/>
       <c r="D19" s="3"/>
@@ -1895,10 +1898,10 @@
     </row>
     <row r="20" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>69</v>
+        <v>63</v>
       </c>
       <c r="C20" s="3"/>
       <c r="D20" s="3"/>
@@ -1915,10 +1918,10 @@
     </row>
     <row r="21" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
-        <v>-1</v>
+        <v>3</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="C21" s="3"/>
       <c r="D21" s="3"/>
@@ -1935,10 +1938,10 @@
     </row>
     <row r="22" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
-        <v>-2</v>
+        <v>100</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>71</v>
+        <v>65</v>
       </c>
       <c r="C22" s="3"/>
       <c r="D22" s="3"/>
@@ -1958,7 +1961,7 @@
         <v>0</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="C23" s="3"/>
       <c r="D23" s="3"/>
@@ -1974,10 +1977,12 @@
       <c r="N23" s="3"/>
     </row>
     <row r="24" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A24" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="B24" s="3"/>
+      <c r="A24" s="1">
+        <v>1</v>
+      </c>
+      <c r="B24" s="3" t="s">
+        <v>67</v>
+      </c>
       <c r="C24" s="3"/>
       <c r="D24" s="3"/>
       <c r="E24" s="3"/>
@@ -1993,10 +1998,10 @@
     </row>
     <row r="25" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A25" s="1">
-        <v>1E-4</v>
+        <v>0</v>
       </c>
       <c r="B25" s="3" t="s">
-        <v>82</v>
+        <v>68</v>
       </c>
       <c r="C25" s="3"/>
       <c r="D25" s="3"/>
@@ -2013,10 +2018,10 @@
     </row>
     <row r="26" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A26" s="1">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>81</v>
+        <v>69</v>
       </c>
       <c r="C26" s="3"/>
       <c r="D26" s="3"/>
@@ -2033,10 +2038,10 @@
     </row>
     <row r="27" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A27" s="1">
-        <v>1</v>
+        <v>-2</v>
       </c>
       <c r="B27" s="3" t="s">
-        <v>80</v>
+        <v>70</v>
       </c>
       <c r="C27" s="3"/>
       <c r="D27" s="3"/>
@@ -2053,10 +2058,10 @@
     </row>
     <row r="28" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A28" s="1">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="B28" s="3" t="s">
-        <v>79</v>
+        <v>71</v>
       </c>
       <c r="C28" s="3"/>
       <c r="D28" s="3"/>
@@ -2072,12 +2077,10 @@
       <c r="N28" s="3"/>
     </row>
     <row r="29" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A29" s="1">
-        <v>1</v>
-      </c>
-      <c r="B29" s="3" t="s">
-        <v>78</v>
-      </c>
+      <c r="A29" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="B29" s="3"/>
       <c r="C29" s="3"/>
       <c r="D29" s="3"/>
       <c r="E29" s="3"/>
@@ -2093,10 +2096,10 @@
     </row>
     <row r="30" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A30" s="1">
-        <v>4</v>
+        <v>1E-4</v>
       </c>
       <c r="B30" s="3" t="s">
-        <v>77</v>
+        <v>81</v>
       </c>
       <c r="C30" s="3"/>
       <c r="D30" s="3"/>
@@ -2113,10 +2116,10 @@
     </row>
     <row r="31" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A31" s="1">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="B31" s="3" t="s">
-        <v>76</v>
+        <v>80</v>
       </c>
       <c r="C31" s="3"/>
       <c r="D31" s="3"/>
@@ -2132,10 +2135,12 @@
       <c r="N31" s="3"/>
     </row>
     <row r="32" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A32" s="3" t="s">
-        <v>83</v>
-      </c>
-      <c r="B32" s="3"/>
+      <c r="A32" s="1">
+        <v>1</v>
+      </c>
+      <c r="B32" s="3" t="s">
+        <v>79</v>
+      </c>
       <c r="C32" s="3"/>
       <c r="D32" s="3"/>
       <c r="E32" s="3"/>
@@ -2151,10 +2156,10 @@
     </row>
     <row r="33" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A33" s="1">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="B33" s="3" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
       <c r="C33" s="3"/>
       <c r="D33" s="3"/>
@@ -2171,10 +2176,10 @@
     </row>
     <row r="34" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A34" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B34" s="3" t="s">
-        <v>84</v>
+        <v>77</v>
       </c>
       <c r="C34" s="3"/>
       <c r="D34" s="3"/>
@@ -2191,10 +2196,10 @@
     </row>
     <row r="35" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A35" s="1">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="B35" s="3" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="C35" s="3"/>
       <c r="D35" s="3"/>
@@ -2211,33 +2216,29 @@
     </row>
     <row r="36" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A36" s="1">
-        <v>123</v>
+        <v>3</v>
       </c>
       <c r="B36" s="3" t="s">
-        <v>105</v>
+        <v>75</v>
       </c>
       <c r="C36" s="3"/>
-      <c r="D36" s="8" t="s">
-        <v>106</v>
-      </c>
-      <c r="E36" s="9"/>
-      <c r="F36" s="9"/>
-      <c r="G36" s="9"/>
-      <c r="H36" s="9"/>
-      <c r="I36" s="9"/>
-      <c r="J36" s="9"/>
-      <c r="K36" s="9"/>
-      <c r="L36" s="9"/>
-      <c r="M36" s="9"/>
-      <c r="N36" s="10"/>
+      <c r="D36" s="3"/>
+      <c r="E36" s="3"/>
+      <c r="F36" s="3"/>
+      <c r="G36" s="3"/>
+      <c r="H36" s="3"/>
+      <c r="I36" s="3"/>
+      <c r="J36" s="3"/>
+      <c r="K36" s="3"/>
+      <c r="L36" s="3"/>
+      <c r="M36" s="3"/>
+      <c r="N36" s="3"/>
     </row>
     <row r="37" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A37" s="7" t="s">
-        <v>103</v>
-      </c>
-      <c r="B37" s="3" t="s">
-        <v>73</v>
-      </c>
+      <c r="A37" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="B37" s="3"/>
       <c r="C37" s="3"/>
       <c r="D37" s="3"/>
       <c r="E37" s="3"/>
@@ -2251,10 +2252,112 @@
       <c r="M37" s="3"/>
       <c r="N37" s="3"/>
     </row>
+    <row r="38" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A38" s="1">
+        <v>0</v>
+      </c>
+      <c r="B38" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="C38" s="3"/>
+      <c r="D38" s="3"/>
+      <c r="E38" s="3"/>
+      <c r="F38" s="3"/>
+      <c r="G38" s="3"/>
+      <c r="H38" s="3"/>
+      <c r="I38" s="3"/>
+      <c r="J38" s="3"/>
+      <c r="K38" s="3"/>
+      <c r="L38" s="3"/>
+      <c r="M38" s="3"/>
+      <c r="N38" s="3"/>
+    </row>
+    <row r="39" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A39" s="1">
+        <v>0</v>
+      </c>
+      <c r="B39" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="C39" s="3"/>
+      <c r="D39" s="3"/>
+      <c r="E39" s="3"/>
+      <c r="F39" s="3"/>
+      <c r="G39" s="3"/>
+      <c r="H39" s="3"/>
+      <c r="I39" s="3"/>
+      <c r="J39" s="3"/>
+      <c r="K39" s="3"/>
+      <c r="L39" s="3"/>
+      <c r="M39" s="3"/>
+      <c r="N39" s="3"/>
+    </row>
+    <row r="40" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A40" s="1">
+        <v>0</v>
+      </c>
+      <c r="B40" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="C40" s="3"/>
+      <c r="D40" s="3"/>
+      <c r="E40" s="3"/>
+      <c r="F40" s="3"/>
+      <c r="G40" s="3"/>
+      <c r="H40" s="3"/>
+      <c r="I40" s="3"/>
+      <c r="J40" s="3"/>
+      <c r="K40" s="3"/>
+      <c r="L40" s="3"/>
+      <c r="M40" s="3"/>
+      <c r="N40" s="3"/>
+    </row>
+    <row r="41" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A41" s="1">
+        <v>123</v>
+      </c>
+      <c r="B41" s="3" t="s">
+        <v>104</v>
+      </c>
+      <c r="C41" s="3"/>
+      <c r="D41" s="8" t="s">
+        <v>105</v>
+      </c>
+      <c r="E41" s="9"/>
+      <c r="F41" s="9"/>
+      <c r="G41" s="9"/>
+      <c r="H41" s="9"/>
+      <c r="I41" s="9"/>
+      <c r="J41" s="9"/>
+      <c r="K41" s="9"/>
+      <c r="L41" s="9"/>
+      <c r="M41" s="9"/>
+      <c r="N41" s="10"/>
+    </row>
+    <row r="42" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A42" s="7" t="s">
+        <v>102</v>
+      </c>
+      <c r="B42" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="C42" s="3"/>
+      <c r="D42" s="3"/>
+      <c r="E42" s="3"/>
+      <c r="F42" s="3"/>
+      <c r="G42" s="3"/>
+      <c r="H42" s="3"/>
+      <c r="I42" s="3"/>
+      <c r="J42" s="3"/>
+      <c r="K42" s="3"/>
+      <c r="L42" s="3"/>
+      <c r="M42" s="3"/>
+      <c r="N42" s="3"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <ignoredErrors>
-    <ignoredError sqref="A37" numberStoredAsText="1"/>
+    <ignoredError sqref="A42" numberStoredAsText="1"/>
   </ignoredErrors>
 </worksheet>
 </file>
@@ -2277,7 +2380,7 @@
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B1" s="3"/>
       <c r="C1" s="3"/>
@@ -2506,7 +2609,7 @@
         <v>1</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C13" s="3"/>
       <c r="D13" s="3"/>
@@ -2637,7 +2740,7 @@
         <v>1</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C20" s="3"/>
       <c r="D20" s="3"/>
@@ -2654,7 +2757,7 @@
         <v>1</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C21" s="3"/>
       <c r="D21" s="3"/>
@@ -2671,7 +2774,7 @@
         <v>0</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C22" s="3"/>
       <c r="D22" s="3"/>
@@ -2722,7 +2825,7 @@
         <v>0.75</v>
       </c>
       <c r="B25" s="3" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C25" s="3"/>
       <c r="D25" s="3"/>
@@ -2739,7 +2842,7 @@
         <v>0</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C26" s="3"/>
       <c r="D26" s="3"/>
@@ -2790,7 +2893,7 @@
         <v>1</v>
       </c>
       <c r="B29" s="3" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C29" s="3"/>
       <c r="D29" s="3"/>
@@ -2807,7 +2910,7 @@
         <v>0</v>
       </c>
       <c r="B30" s="3" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C30" s="3"/>
       <c r="D30" s="3"/>
@@ -2824,7 +2927,7 @@
         <v>1</v>
       </c>
       <c r="B31" s="3" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C31" s="3"/>
       <c r="D31" s="3"/>
@@ -3019,7 +3122,7 @@
     </row>
     <row r="43" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A43" s="3" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B43" s="3"/>
       <c r="C43" s="3"/>
@@ -3034,10 +3137,10 @@
     </row>
     <row r="44" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A44" s="3" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B44" s="3" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C44" s="3"/>
       <c r="D44" s="3"/>
@@ -3051,10 +3154,10 @@
     </row>
     <row r="45" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A45" s="3" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B45" s="3" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C45" s="3"/>
       <c r="D45" s="3"/>
@@ -3068,10 +3171,10 @@
     </row>
     <row r="46" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A46" s="3" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B46" s="3" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C46" s="3"/>
       <c r="D46" s="3"/>
@@ -3085,7 +3188,7 @@
     </row>
     <row r="47" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A47" s="3" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B47" s="3"/>
       <c r="C47" s="3"/>
@@ -3365,7 +3468,7 @@
         <v>999</v>
       </c>
       <c r="B64" s="3" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C64" s="3"/>
       <c r="D64" s="3"/>

</xml_diff>

<commit_message>
#80120: Document F_std_basis multiyr option in helper spreadsheets
</commit_message>
<xml_diff>
--- a/Helper_Spreadsheets/SS_330_starter_and_forecast_helper.xlsx
+++ b/Helper_Spreadsheets/SS_330_starter_and_forecast_helper.xlsx
@@ -242,9 +242,6 @@
   </si>
   <si>
     <t># ALK tolerance (example 0.0001)</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> # F_report_basis: 0=raw; 1=F/Fspr; 2=F/Fmsy ; 3=F/Fbtgt</t>
   </si>
   <si>
     <t># F_report_units: 0=skip; 1=exploitation(Bio); 2=exploitation(Num); 3=sum(Frates); 4=true F (=Z-M) for range of ages</t>
@@ -379,6 +376,9 @@
   </si>
   <si>
     <t># Following COND lines only if detailed output = 3:</t>
+  </si>
+  <si>
+    <t># F_std_basis: 0=raw_annual_F; 1=F/Fspr; 2=F/Fmsy; 3=F/Fbtgt; where F means annual_F; values &gt;=11 invoke multiyr with 10's digit</t>
   </si>
 </sst>
 </file>
@@ -1538,7 +1538,7 @@
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B1" s="3"/>
       <c r="C1" s="3"/>
@@ -1711,7 +1711,7 @@
         <v>1</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C10" s="3"/>
       <c r="D10" s="3"/>
@@ -1728,7 +1728,7 @@
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B11" s="3"/>
       <c r="C11" s="3"/>
@@ -1746,7 +1746,7 @@
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B12" s="3"/>
       <c r="C12" s="3"/>
@@ -1764,7 +1764,7 @@
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B13" s="3"/>
       <c r="C13" s="3"/>
@@ -1782,7 +1782,7 @@
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B14" s="3"/>
       <c r="C14" s="3"/>
@@ -1800,7 +1800,7 @@
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B15" s="3"/>
       <c r="C15" s="3"/>
@@ -2099,7 +2099,7 @@
         <v>1E-4</v>
       </c>
       <c r="B30" s="3" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C30" s="3"/>
       <c r="D30" s="3"/>
@@ -2119,7 +2119,7 @@
         <v>0</v>
       </c>
       <c r="B31" s="3" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C31" s="3"/>
       <c r="D31" s="3"/>
@@ -2139,7 +2139,7 @@
         <v>1</v>
       </c>
       <c r="B32" s="3" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C32" s="3"/>
       <c r="D32" s="3"/>
@@ -2159,7 +2159,7 @@
         <v>2</v>
       </c>
       <c r="B33" s="3" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C33" s="3"/>
       <c r="D33" s="3"/>
@@ -2179,7 +2179,7 @@
         <v>1</v>
       </c>
       <c r="B34" s="3" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C34" s="3"/>
       <c r="D34" s="3"/>
@@ -2199,7 +2199,7 @@
         <v>4</v>
       </c>
       <c r="B35" s="3" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C35" s="3"/>
       <c r="D35" s="3"/>
@@ -2219,7 +2219,7 @@
         <v>3</v>
       </c>
       <c r="B36" s="3" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C36" s="3"/>
       <c r="D36" s="3"/>
@@ -2236,7 +2236,7 @@
     </row>
     <row r="37" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A37" s="3" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B37" s="3"/>
       <c r="C37" s="3"/>
@@ -2257,7 +2257,7 @@
         <v>0</v>
       </c>
       <c r="B38" s="3" t="s">
-        <v>74</v>
+        <v>111</v>
       </c>
       <c r="C38" s="3"/>
       <c r="D38" s="3"/>
@@ -2277,7 +2277,7 @@
         <v>0</v>
       </c>
       <c r="B39" s="3" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C39" s="3"/>
       <c r="D39" s="3"/>
@@ -2317,11 +2317,11 @@
         <v>123</v>
       </c>
       <c r="B41" s="3" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C41" s="3"/>
       <c r="D41" s="8" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E41" s="9"/>
       <c r="F41" s="9"/>
@@ -2336,7 +2336,7 @@
     </row>
     <row r="42" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A42" s="7" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B42" s="3" t="s">
         <v>72</v>
@@ -2356,6 +2356,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
   <ignoredErrors>
     <ignoredError sqref="A42" numberStoredAsText="1"/>
   </ignoredErrors>
@@ -2380,7 +2381,7 @@
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B1" s="3"/>
       <c r="C1" s="3"/>
@@ -2609,7 +2610,7 @@
         <v>1</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C13" s="3"/>
       <c r="D13" s="3"/>
@@ -2740,7 +2741,7 @@
         <v>1</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C20" s="3"/>
       <c r="D20" s="3"/>
@@ -2757,7 +2758,7 @@
         <v>1</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C21" s="3"/>
       <c r="D21" s="3"/>
@@ -2774,7 +2775,7 @@
         <v>0</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C22" s="3"/>
       <c r="D22" s="3"/>
@@ -2825,7 +2826,7 @@
         <v>0.75</v>
       </c>
       <c r="B25" s="3" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C25" s="3"/>
       <c r="D25" s="3"/>
@@ -2842,7 +2843,7 @@
         <v>0</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C26" s="3"/>
       <c r="D26" s="3"/>
@@ -2893,7 +2894,7 @@
         <v>1</v>
       </c>
       <c r="B29" s="3" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C29" s="3"/>
       <c r="D29" s="3"/>
@@ -2910,7 +2911,7 @@
         <v>0</v>
       </c>
       <c r="B30" s="3" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C30" s="3"/>
       <c r="D30" s="3"/>
@@ -2927,7 +2928,7 @@
         <v>1</v>
       </c>
       <c r="B31" s="3" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C31" s="3"/>
       <c r="D31" s="3"/>
@@ -3122,7 +3123,7 @@
     </row>
     <row r="43" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A43" s="3" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B43" s="3"/>
       <c r="C43" s="3"/>
@@ -3137,10 +3138,10 @@
     </row>
     <row r="44" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A44" s="3" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B44" s="3" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C44" s="3"/>
       <c r="D44" s="3"/>
@@ -3154,10 +3155,10 @@
     </row>
     <row r="45" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A45" s="3" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B45" s="3" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C45" s="3"/>
       <c r="D45" s="3"/>
@@ -3171,10 +3172,10 @@
     </row>
     <row r="46" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A46" s="3" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B46" s="3" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C46" s="3"/>
       <c r="D46" s="3"/>
@@ -3188,7 +3189,7 @@
     </row>
     <row r="47" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A47" s="3" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B47" s="3"/>
       <c r="C47" s="3"/>
@@ -3468,7 +3469,7 @@
         <v>999</v>
       </c>
       <c r="B64" s="3" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C64" s="3"/>
       <c r="D64" s="3"/>

</xml_diff>

<commit_message>
manual, helper: issue #10: describe hcr option 0
</commit_message>
<xml_diff>
--- a/Helper_Spreadsheets/SS_330_starter_and_forecast_helper.xlsx
+++ b/Helper_Spreadsheets/SS_330_starter_and_forecast_helper.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Kathryn.Doering\Documents\Documents\Stock_Synthesis\vlab_repo\SS_documentation\ss_documentation\Helper_Spreadsheets\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Kathryn.Doering\Documents\Documents\Stock_Synthesis\nmfs-stock-synthesis-repos\ss-documentation\Helper_Spreadsheets\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="112">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="113">
   <si>
     <t>#</t>
   </si>
@@ -275,9 +275,6 @@
   </si>
   <si>
     <t># Forecast selectivity (0=fcast selex is mean from year range; 1=fcast selectivity from annual time-vary parms)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">#Control rule method (1: ramp does catch=f(SSB), buffer on F; 2: ramp does F=f(SSB), buffer on F; </t>
   </si>
   <si>
     <t>3: ramp does catch=f(SSB), buffer on catch; 4: ramp does F=f(SSB), buffer on catch)</t>
@@ -379,6 +376,12 @@
   </si>
   <si>
     <t># F_std_basis: 0=raw_annual_F; 1=F/Fspr; 2=F/Fmsy; 3=F/Fbtgt; where F means annual_F; values &gt;=11 invoke multiyr with 10's digit</t>
+  </si>
+  <si>
+    <t>#Control rule method (0:none, 1: ramp does catch=f(SSB), buffer on F; 2: ramp does F=f(SSB), buffer on F; )</t>
+  </si>
+  <si>
+    <t>Control rule method 0 (none) available as of 3.30.17. Ignores the additional control rule inputs below it.</t>
   </si>
 </sst>
 </file>
@@ -1538,7 +1541,7 @@
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B1" s="3"/>
       <c r="C1" s="3"/>
@@ -1711,7 +1714,7 @@
         <v>1</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C10" s="3"/>
       <c r="D10" s="3"/>
@@ -1728,7 +1731,7 @@
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B11" s="3"/>
       <c r="C11" s="3"/>
@@ -1746,7 +1749,7 @@
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B12" s="3"/>
       <c r="C12" s="3"/>
@@ -1764,7 +1767,7 @@
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B13" s="3"/>
       <c r="C13" s="3"/>
@@ -1782,7 +1785,7 @@
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B14" s="3"/>
       <c r="C14" s="3"/>
@@ -1800,7 +1803,7 @@
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B15" s="3"/>
       <c r="C15" s="3"/>
@@ -2257,7 +2260,7 @@
         <v>0</v>
       </c>
       <c r="B38" s="3" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C38" s="3"/>
       <c r="D38" s="3"/>
@@ -2317,11 +2320,11 @@
         <v>123</v>
       </c>
       <c r="B41" s="3" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C41" s="3"/>
       <c r="D41" s="8" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="E41" s="9"/>
       <c r="F41" s="9"/>
@@ -2336,7 +2339,7 @@
     </row>
     <row r="42" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A42" s="7" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B42" s="3" t="s">
         <v>72</v>
@@ -2365,10 +2368,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K64"/>
+  <dimension ref="A1:U64"/>
   <sheetViews>
-    <sheetView topLeftCell="A43" workbookViewId="0">
-      <selection activeCell="C70" sqref="C70"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="W18" sqref="W18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2381,7 +2384,7 @@
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B1" s="3"/>
       <c r="C1" s="3"/>
@@ -2610,7 +2613,7 @@
         <v>1</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C13" s="3"/>
       <c r="D13" s="3"/>
@@ -2671,7 +2674,7 @@
       <c r="J16" s="3"/>
       <c r="K16" s="6"/>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="s">
         <v>36</v>
       </c>
@@ -2696,7 +2699,7 @@
       <c r="J17" s="3"/>
       <c r="K17" s="6"/>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
         <v>0</v>
       </c>
@@ -2721,7 +2724,7 @@
       <c r="J18" s="3"/>
       <c r="K18" s="6"/>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
         <v>0</v>
       </c>
@@ -2736,7 +2739,7 @@
       <c r="J19" s="3"/>
       <c r="K19" s="6"/>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
         <v>1</v>
       </c>
@@ -2753,12 +2756,12 @@
       <c r="J20" s="3"/>
       <c r="K20" s="6"/>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
         <v>1</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>85</v>
+        <v>111</v>
       </c>
       <c r="C21" s="3"/>
       <c r="D21" s="3"/>
@@ -2769,13 +2772,25 @@
       <c r="I21" s="3"/>
       <c r="J21" s="3"/>
       <c r="K21" s="6"/>
-    </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L21" s="8" t="s">
+        <v>112</v>
+      </c>
+      <c r="M21" s="9"/>
+      <c r="N21" s="9"/>
+      <c r="O21" s="9"/>
+      <c r="P21" s="9"/>
+      <c r="Q21" s="9"/>
+      <c r="R21" s="9"/>
+      <c r="S21" s="9"/>
+      <c r="T21" s="9"/>
+      <c r="U21" s="10"/>
+    </row>
+    <row r="22" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A22" s="3" t="s">
         <v>0</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C22" s="3"/>
       <c r="D22" s="3"/>
@@ -2787,7 +2802,7 @@
       <c r="J22" s="3"/>
       <c r="K22" s="6"/>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A23" s="1">
         <v>0.4</v>
       </c>
@@ -2804,7 +2819,7 @@
       <c r="J23" s="3"/>
       <c r="K23" s="6"/>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A24" s="1">
         <v>0.1</v>
       </c>
@@ -2821,12 +2836,12 @@
       <c r="J24" s="3"/>
       <c r="K24" s="6"/>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A25" s="1">
         <v>0.75</v>
       </c>
       <c r="B25" s="3" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C25" s="3"/>
       <c r="D25" s="3"/>
@@ -2838,12 +2853,12 @@
       <c r="J25" s="3"/>
       <c r="K25" s="6"/>
     </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A26" s="3" t="s">
         <v>0</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C26" s="3"/>
       <c r="D26" s="3"/>
@@ -2855,7 +2870,7 @@
       <c r="J26" s="3"/>
       <c r="K26" s="6"/>
     </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A27" s="1">
         <v>3</v>
       </c>
@@ -2872,7 +2887,7 @@
       <c r="J27" s="3"/>
       <c r="K27" s="6"/>
     </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A28" s="1">
         <v>3</v>
       </c>
@@ -2889,12 +2904,12 @@
       <c r="J28" s="3"/>
       <c r="K28" s="6"/>
     </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A29" s="1">
         <v>1</v>
       </c>
       <c r="B29" s="3" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C29" s="3"/>
       <c r="D29" s="3"/>
@@ -2906,12 +2921,12 @@
       <c r="J29" s="3"/>
       <c r="K29" s="6"/>
     </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A30" s="3" t="s">
         <v>0</v>
       </c>
       <c r="B30" s="3" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C30" s="3"/>
       <c r="D30" s="3"/>
@@ -2923,12 +2938,12 @@
       <c r="J30" s="3"/>
       <c r="K30" s="6"/>
     </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A31" s="1">
         <v>1</v>
       </c>
       <c r="B31" s="3" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C31" s="3"/>
       <c r="D31" s="3"/>
@@ -2940,7 +2955,7 @@
       <c r="J31" s="3"/>
       <c r="K31" s="6"/>
     </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A32" s="1">
         <v>0</v>
       </c>
@@ -3123,7 +3138,7 @@
     </row>
     <row r="43" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A43" s="3" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B43" s="3"/>
       <c r="C43" s="3"/>
@@ -3138,10 +3153,10 @@
     </row>
     <row r="44" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A44" s="3" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B44" s="3" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C44" s="3"/>
       <c r="D44" s="3"/>
@@ -3155,10 +3170,10 @@
     </row>
     <row r="45" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A45" s="3" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B45" s="3" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C45" s="3"/>
       <c r="D45" s="3"/>
@@ -3172,10 +3187,10 @@
     </row>
     <row r="46" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A46" s="3" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B46" s="3" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C46" s="3"/>
       <c r="D46" s="3"/>
@@ -3189,7 +3204,7 @@
     </row>
     <row r="47" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A47" s="3" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B47" s="3"/>
       <c r="C47" s="3"/>

</xml_diff>

<commit_message>
manual, helper: #15: add -999 definition
</commit_message>
<xml_diff>
--- a/Helper_Spreadsheets/SS_330_starter_and_forecast_helper.xlsx
+++ b/Helper_Spreadsheets/SS_330_starter_and_forecast_helper.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="113">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="114">
   <si>
     <t>#</t>
   </si>
@@ -382,6 +382,9 @@
   </si>
   <si>
     <t>Control rule method 0 (none) available as of 3.30.17. Ignores the additional control rule inputs below it.</t>
+  </si>
+  <si>
+    <t>-999 indicates the start year of the model</t>
   </si>
 </sst>
 </file>
@@ -487,7 +490,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
@@ -503,6 +506,9 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2371,7 +2377,7 @@
   <dimension ref="A1:U64"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="W18" sqref="W18"/>
+      <selection activeCell="G23" sqref="G23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2701,7 +2707,7 @@
     </row>
     <row r="18" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
-        <v>0</v>
+        <v>-999</v>
       </c>
       <c r="B18" s="1">
         <v>0</v>
@@ -2718,10 +2724,12 @@
       <c r="F18" s="1">
         <v>2016</v>
       </c>
-      <c r="G18" s="3"/>
-      <c r="H18" s="3"/>
-      <c r="I18" s="3"/>
-      <c r="J18" s="3"/>
+      <c r="G18" s="11" t="s">
+        <v>113</v>
+      </c>
+      <c r="H18" s="12"/>
+      <c r="I18" s="12"/>
+      <c r="J18" s="13"/>
       <c r="K18" s="6"/>
     </row>
     <row r="19" spans="1:21" x14ac:dyDescent="0.25">
@@ -3498,6 +3506,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
manual, helper, #38: doc log scale options for F, bratio
</commit_message>
<xml_diff>
--- a/Helper_Spreadsheets/SS_330_starter_and_forecast_helper.xlsx
+++ b/Helper_Spreadsheets/SS_330_starter_and_forecast_helper.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="340" uniqueCount="124">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="340" uniqueCount="125">
   <si>
     <t>#</t>
   </si>
@@ -255,9 +255,6 @@
   </si>
   <si>
     <t># Fraction (X) for Depletion denominator (e.g. 0.4)</t>
-  </si>
-  <si>
-    <t># Depletion basis:  denom is: 0=skip; 1=rel X*B0; 2=rel X*Bmsy; 3=rel X*B_styr</t>
   </si>
   <si>
     <t># min age for calc of summary biomass</t>
@@ -379,9 +376,6 @@
     <t># Following COND lines only if detailed output = 3:</t>
   </si>
   <si>
-    <t># F_std_basis: 0=raw_annual_F; 1=F/Fspr; 2=F/Fmsy; 3=F/Fbtgt; where F means annual_F; values &gt;=11 invoke multiyr with 10's digit</t>
-  </si>
-  <si>
     <t>#Control rule method (0:none, 1: ramp does catch=f(SSB), buffer on F; 2: ramp does F=f(SSB), buffer on F; )</t>
   </si>
   <si>
@@ -419,6 +413,15 @@
   </si>
   <si>
     <t>see additonal forecast tabs for specific types of forecast examples</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> # Depletion basis: denom is: 0=skip; 1=rel XSPB0; 2=rel SPBmsy; 3=rel XSPB_styr; 4=rel X*SPB_endyr; values &gt;=11 invoke N multiyr (up to 9!) with 10's digit; &gt;100 invokes log(ratio)</t>
+  </si>
+  <si>
+    <t># F_std_basis: 0=raw_annual_F; 1=F/Fspr; 2=F/Fmsy; 3=F/Fbtgt; where F means annual_F; values &gt;=11 invoke N multiyr (up o 9) with 10's digit; &gt;100 invokes log(ratio)</t>
+  </si>
+  <si>
+    <t>#V3.30.17.00-safe;_2021_05_25;_Stock_Synthesis_by_Richard_Methot_(NOAA)_using_ADMB_12.3</t>
   </si>
 </sst>
 </file>
@@ -640,9 +643,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -652,6 +652,15 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -659,12 +668,6 @@
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1705,7 +1708,7 @@
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
-        <v>99</v>
+        <v>124</v>
       </c>
       <c r="B1" s="3"/>
       <c r="C1" s="3"/>
@@ -1878,7 +1881,7 @@
         <v>1</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C10" s="3"/>
       <c r="D10" s="3"/>
@@ -1895,7 +1898,7 @@
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B11" s="3"/>
       <c r="C11" s="3"/>
@@ -1913,7 +1916,7 @@
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B12" s="3"/>
       <c r="C12" s="3"/>
@@ -1931,7 +1934,7 @@
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B13" s="3"/>
       <c r="C13" s="3"/>
@@ -1949,7 +1952,7 @@
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B14" s="3"/>
       <c r="C14" s="3"/>
@@ -1967,7 +1970,7 @@
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B15" s="3"/>
       <c r="C15" s="3"/>
@@ -2266,7 +2269,7 @@
         <v>1E-4</v>
       </c>
       <c r="B30" s="3" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C30" s="3"/>
       <c r="D30" s="3"/>
@@ -2286,7 +2289,7 @@
         <v>0</v>
       </c>
       <c r="B31" s="3" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C31" s="3"/>
       <c r="D31" s="3"/>
@@ -2306,7 +2309,7 @@
         <v>1</v>
       </c>
       <c r="B32" s="3" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C32" s="3"/>
       <c r="D32" s="3"/>
@@ -2326,7 +2329,7 @@
         <v>2</v>
       </c>
       <c r="B33" s="3" t="s">
-        <v>77</v>
+        <v>122</v>
       </c>
       <c r="C33" s="3"/>
       <c r="D33" s="3"/>
@@ -2403,7 +2406,7 @@
     </row>
     <row r="37" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A37" s="3" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B37" s="3"/>
       <c r="C37" s="3"/>
@@ -2424,7 +2427,7 @@
         <v>0</v>
       </c>
       <c r="B38" s="3" t="s">
-        <v>110</v>
+        <v>123</v>
       </c>
       <c r="C38" s="3"/>
       <c r="D38" s="3"/>
@@ -2444,7 +2447,7 @@
         <v>0</v>
       </c>
       <c r="B39" s="3" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C39" s="3"/>
       <c r="D39" s="3"/>
@@ -2484,11 +2487,11 @@
         <v>123</v>
       </c>
       <c r="B41" s="3" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C41" s="3"/>
       <c r="D41" s="8" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="E41" s="9"/>
       <c r="F41" s="9"/>
@@ -2503,7 +2506,7 @@
     </row>
     <row r="42" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A42" s="7" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B42" s="3" t="s">
         <v>72</v>
@@ -2548,7 +2551,7 @@
   <sheetData>
     <row r="1" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B1" s="3"/>
       <c r="C1" s="3"/>
@@ -2559,7 +2562,7 @@
       <c r="H1" s="3"/>
       <c r="I1" s="3"/>
       <c r="J1" s="8" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="K1" s="14"/>
       <c r="L1" s="9"/>
@@ -2784,7 +2787,7 @@
         <v>1</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C13" s="3"/>
       <c r="D13" s="3"/>
@@ -2890,7 +2893,7 @@
         <v>2016</v>
       </c>
       <c r="G18" s="11" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="H18" s="12"/>
       <c r="I18" s="12"/>
@@ -2917,7 +2920,7 @@
         <v>1</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C20" s="3"/>
       <c r="D20" s="3"/>
@@ -2934,7 +2937,7 @@
         <v>1</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="C21" s="3"/>
       <c r="D21" s="3"/>
@@ -2946,7 +2949,7 @@
       <c r="J21" s="3"/>
       <c r="K21" s="6"/>
       <c r="L21" s="8" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="M21" s="9"/>
       <c r="N21" s="9"/>
@@ -2963,7 +2966,7 @@
         <v>0</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C22" s="3"/>
       <c r="D22" s="3"/>
@@ -3014,7 +3017,7 @@
         <v>0.75</v>
       </c>
       <c r="B25" s="3" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C25" s="3"/>
       <c r="D25" s="3"/>
@@ -3031,7 +3034,7 @@
         <v>0</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C26" s="3"/>
       <c r="D26" s="3"/>
@@ -3082,7 +3085,7 @@
         <v>1</v>
       </c>
       <c r="B29" s="3" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C29" s="3"/>
       <c r="D29" s="3"/>
@@ -3099,7 +3102,7 @@
         <v>0</v>
       </c>
       <c r="B30" s="3" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C30" s="3"/>
       <c r="D30" s="3"/>
@@ -3116,7 +3119,7 @@
         <v>1</v>
       </c>
       <c r="B31" s="3" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C31" s="3"/>
       <c r="D31" s="3"/>
@@ -3311,7 +3314,7 @@
     </row>
     <row r="43" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A43" s="3" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B43" s="3"/>
       <c r="C43" s="3"/>
@@ -3326,10 +3329,10 @@
     </row>
     <row r="44" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A44" s="3" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B44" s="3" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C44" s="3"/>
       <c r="D44" s="3"/>
@@ -3343,10 +3346,10 @@
     </row>
     <row r="45" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A45" s="3" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B45" s="3" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C45" s="3"/>
       <c r="D45" s="3"/>
@@ -3360,10 +3363,10 @@
     </row>
     <row r="46" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A46" s="3" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B46" s="3" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C46" s="3"/>
       <c r="D46" s="3"/>
@@ -3377,7 +3380,7 @@
     </row>
     <row r="47" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A47" s="3" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B47" s="3"/>
       <c r="C47" s="3"/>
@@ -3657,7 +3660,7 @@
         <v>999</v>
       </c>
       <c r="B64" s="3" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C64" s="3"/>
       <c r="D64" s="3"/>
@@ -3691,7 +3694,7 @@
   <sheetData>
     <row r="1" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="B1" s="3"/>
       <c r="C1" s="3"/>
@@ -3746,7 +3749,7 @@
       <c r="E4" s="3"/>
       <c r="F4" s="3"/>
       <c r="G4" s="8" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="H4" s="9"/>
       <c r="I4" s="9"/>
@@ -3924,13 +3927,13 @@
         <v>-1</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C13" s="3"/>
       <c r="D13" s="3"/>
       <c r="E13" s="3"/>
       <c r="F13" s="23" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="G13" s="24"/>
       <c r="H13" s="24"/>
@@ -3944,7 +3947,7 @@
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A14" s="26" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="B14" s="27"/>
       <c r="C14" s="27"/>
@@ -4827,7 +4830,7 @@
   <sheetData>
     <row r="1" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="B1" s="3"/>
       <c r="C1" s="3"/>
@@ -5128,7 +5131,7 @@
         <v>-1</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C13" s="3"/>
       <c r="D13" s="3"/>
@@ -5142,7 +5145,7 @@
       <c r="L13" s="3"/>
       <c r="M13" s="3"/>
       <c r="N13" s="8" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="O13" s="9"/>
       <c r="P13" s="9"/>
@@ -5150,7 +5153,7 @@
     </row>
     <row r="14" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A14" s="26" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="B14" s="27"/>
       <c r="C14" s="27"/>
@@ -5986,7 +5989,7 @@
   <sheetData>
     <row r="1" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="B1" s="3"/>
       <c r="C1" s="3"/>
@@ -6287,7 +6290,7 @@
         <v>1</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C13" s="3"/>
       <c r="D13" s="3"/>
@@ -6460,7 +6463,7 @@
         <v>1</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C20" s="3"/>
       <c r="D20" s="3"/>
@@ -6483,7 +6486,7 @@
         <v>0</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="C21" s="3"/>
       <c r="D21" s="3"/>
@@ -6495,7 +6498,7 @@
       <c r="J21" s="3"/>
       <c r="K21" s="6"/>
       <c r="L21" s="8" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="M21" s="9"/>
       <c r="N21" s="9"/>
@@ -6508,7 +6511,7 @@
         <v>0</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C22" s="3"/>
       <c r="D22" s="3"/>
@@ -6542,14 +6545,14 @@
       <c r="I23" s="3"/>
       <c r="J23" s="3"/>
       <c r="K23" s="6"/>
-      <c r="L23" s="32" t="s">
-        <v>120</v>
-      </c>
-      <c r="M23" s="33"/>
-      <c r="N23" s="33"/>
-      <c r="O23" s="33"/>
-      <c r="P23" s="33"/>
-      <c r="Q23" s="34"/>
+      <c r="L23" s="31" t="s">
+        <v>118</v>
+      </c>
+      <c r="M23" s="32"/>
+      <c r="N23" s="32"/>
+      <c r="O23" s="32"/>
+      <c r="P23" s="32"/>
+      <c r="Q23" s="33"/>
     </row>
     <row r="24" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A24" s="1">
@@ -6567,19 +6570,19 @@
       <c r="I24" s="3"/>
       <c r="J24" s="3"/>
       <c r="K24" s="6"/>
-      <c r="L24" s="38"/>
-      <c r="M24" s="31"/>
-      <c r="N24" s="31"/>
-      <c r="O24" s="31"/>
-      <c r="P24" s="31"/>
-      <c r="Q24" s="39"/>
+      <c r="L24" s="34"/>
+      <c r="M24" s="35"/>
+      <c r="N24" s="35"/>
+      <c r="O24" s="35"/>
+      <c r="P24" s="35"/>
+      <c r="Q24" s="36"/>
     </row>
     <row r="25" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A25" s="1">
         <v>1</v>
       </c>
       <c r="B25" s="3" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C25" s="3"/>
       <c r="D25" s="3"/>
@@ -6590,19 +6593,19 @@
       <c r="I25" s="3"/>
       <c r="J25" s="3"/>
       <c r="K25" s="6"/>
-      <c r="L25" s="35"/>
-      <c r="M25" s="36"/>
-      <c r="N25" s="36"/>
-      <c r="O25" s="36"/>
-      <c r="P25" s="36"/>
-      <c r="Q25" s="37"/>
+      <c r="L25" s="37"/>
+      <c r="M25" s="38"/>
+      <c r="N25" s="38"/>
+      <c r="O25" s="38"/>
+      <c r="P25" s="38"/>
+      <c r="Q25" s="39"/>
     </row>
     <row r="26" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A26" s="3" t="s">
         <v>0</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C26" s="3"/>
       <c r="D26" s="3"/>
@@ -6671,7 +6674,7 @@
         <v>1</v>
       </c>
       <c r="B29" s="3" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C29" s="3"/>
       <c r="D29" s="3"/>
@@ -6694,7 +6697,7 @@
         <v>0</v>
       </c>
       <c r="B30" s="3" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C30" s="3"/>
       <c r="D30" s="3"/>
@@ -6717,7 +6720,7 @@
         <v>1</v>
       </c>
       <c r="B31" s="3" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C31" s="3"/>
       <c r="D31" s="3"/>
@@ -6984,7 +6987,7 @@
     </row>
     <row r="43" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A43" s="3" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B43" s="3"/>
       <c r="C43" s="3"/>
@@ -7005,10 +7008,10 @@
     </row>
     <row r="44" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A44" s="3" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B44" s="3" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C44" s="3"/>
       <c r="D44" s="3"/>
@@ -7028,10 +7031,10 @@
     </row>
     <row r="45" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A45" s="3" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B45" s="3" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C45" s="3"/>
       <c r="D45" s="3"/>
@@ -7051,10 +7054,10 @@
     </row>
     <row r="46" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A46" s="3" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B46" s="3" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C46" s="3"/>
       <c r="D46" s="3"/>
@@ -7074,7 +7077,7 @@
     </row>
     <row r="47" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A47" s="3" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B47" s="3"/>
       <c r="C47" s="3"/>
@@ -7456,7 +7459,7 @@
         <v>999</v>
       </c>
       <c r="B64" s="3" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C64" s="3"/>
       <c r="D64" s="3"/>
@@ -7494,7 +7497,7 @@
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B1" s="3"/>
       <c r="C1" s="3"/>
@@ -7747,7 +7750,7 @@
         <v>1</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C13" s="3"/>
       <c r="D13" s="3"/>
@@ -7863,7 +7866,7 @@
         <v>2016</v>
       </c>
       <c r="G18" s="11" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="H18" s="12"/>
       <c r="I18" s="12"/>
@@ -7894,7 +7897,7 @@
         <v>1</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C20" s="3"/>
       <c r="D20" s="3"/>
@@ -7913,7 +7916,7 @@
         <v>1</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="C21" s="3"/>
       <c r="D21" s="3"/>
@@ -7932,7 +7935,7 @@
         <v>0</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C22" s="3"/>
       <c r="D22" s="3"/>
@@ -7989,7 +7992,7 @@
         <v>0.75</v>
       </c>
       <c r="B25" s="3" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C25" s="3"/>
       <c r="D25" s="3"/>
@@ -8008,7 +8011,7 @@
         <v>0</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C26" s="3"/>
       <c r="D26" s="3"/>
@@ -8065,7 +8068,7 @@
         <v>1</v>
       </c>
       <c r="B29" s="3" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C29" s="3"/>
       <c r="D29" s="3"/>
@@ -8084,7 +8087,7 @@
         <v>0</v>
       </c>
       <c r="B30" s="3" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C30" s="3"/>
       <c r="D30" s="3"/>
@@ -8103,7 +8106,7 @@
         <v>1</v>
       </c>
       <c r="B31" s="3" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C31" s="3"/>
       <c r="D31" s="3"/>
@@ -8322,7 +8325,7 @@
     </row>
     <row r="43" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A43" s="3" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B43" s="3"/>
       <c r="C43" s="3"/>
@@ -8339,10 +8342,10 @@
     </row>
     <row r="44" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A44" s="3" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B44" s="3" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C44" s="3"/>
       <c r="D44" s="3"/>
@@ -8358,10 +8361,10 @@
     </row>
     <row r="45" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A45" s="3" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B45" s="3" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C45" s="3"/>
       <c r="D45" s="3"/>
@@ -8377,10 +8380,10 @@
     </row>
     <row r="46" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A46" s="3" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B46" s="3" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C46" s="3"/>
       <c r="D46" s="3"/>
@@ -8396,7 +8399,7 @@
     </row>
     <row r="47" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A47" s="3" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B47" s="3"/>
       <c r="C47" s="3"/>
@@ -8680,7 +8683,7 @@
       </c>
       <c r="E62" s="3"/>
       <c r="F62" s="8" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="G62" s="9"/>
       <c r="H62" s="9"/>
@@ -8804,7 +8807,7 @@
         <v>999</v>
       </c>
       <c r="B68" s="3" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C68" s="3"/>
       <c r="D68" s="3"/>

</xml_diff>

<commit_message>
helper, issue #57: document F at b lim input
</commit_message>
<xml_diff>
--- a/Helper_Spreadsheets/SS_330_starter_and_forecast_helper.xlsx
+++ b/Helper_Spreadsheets/SS_330_starter_and_forecast_helper.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Kathryn.Doering\Documents\Documents\Stock_Synthesis\nmfs-stock-synthesis-repos\ss-documentation\Helper_Spreadsheets\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Kathryn.Doering\Documents\github_repos\ss-documentation\Helper_Spreadsheets\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="340" uniqueCount="125">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="342" uniqueCount="129">
   <si>
     <t>#</t>
   </si>
@@ -422,6 +422,18 @@
   </si>
   <si>
     <t>#V3.30.17.00-safe;_2021_05_25;_Stock_Synthesis_by_Richard_Methot_(NOAA)_using_ADMB_12.3</t>
+  </si>
+  <si>
+    <t># Benchmarks: 0=skip; 1=calc F_spr,F_btgt,F_msy; 2=calc F_spr,F0.1,F_msy; 3=add F_Blimit</t>
+  </si>
+  <si>
+    <t># -0.25 # COND: if Benchmarks = 3; Blimit as a fraction of Bmsy (neg value to use as frac of Bzerio)</t>
+  </si>
+  <si>
+    <t>3 available as of 3.30.18</t>
+  </si>
+  <si>
+    <t>#V3.30.18.00-safe;_2021_10_xx;_Stock_Synthesis_by_Richard_Methot_(NOAA)_using_ADMB_12.0</t>
   </si>
 </sst>
 </file>
@@ -478,7 +490,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="12">
+  <borders count="14">
     <border>
       <left/>
       <right/>
@@ -603,11 +615,37 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="40">
+  <cellXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
@@ -670,6 +708,9 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -678,8 +719,8 @@
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
+      <color rgb="FFFFFF99"/>
       <color rgb="FFBEFCFE"/>
-      <color rgb="FFFFFF99"/>
       <color rgb="FFA3FDF4"/>
       <color rgb="FFFFFFFF"/>
       <color rgb="FFAFF1F1"/>
@@ -709,7 +750,7 @@
     <xdr:to>
       <xdr:col>18</xdr:col>
       <xdr:colOff>66675</xdr:colOff>
-      <xdr:row>9</xdr:row>
+      <xdr:row>10</xdr:row>
       <xdr:rowOff>142875</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -790,13 +831,13 @@
     <xdr:from>
       <xdr:col>11</xdr:col>
       <xdr:colOff>285750</xdr:colOff>
-      <xdr:row>9</xdr:row>
+      <xdr:row>10</xdr:row>
       <xdr:rowOff>142875</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>18</xdr:col>
       <xdr:colOff>381000</xdr:colOff>
-      <xdr:row>19</xdr:row>
+      <xdr:row>20</xdr:row>
       <xdr:rowOff>57150</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -941,13 +982,13 @@
     <xdr:from>
       <xdr:col>12</xdr:col>
       <xdr:colOff>123825</xdr:colOff>
-      <xdr:row>37</xdr:row>
+      <xdr:row>38</xdr:row>
       <xdr:rowOff>95249</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>19</xdr:col>
       <xdr:colOff>219075</xdr:colOff>
-      <xdr:row>46</xdr:row>
+      <xdr:row>47</xdr:row>
       <xdr:rowOff>38100</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -1100,13 +1141,13 @@
     <xdr:from>
       <xdr:col>3</xdr:col>
       <xdr:colOff>190500</xdr:colOff>
-      <xdr:row>18</xdr:row>
+      <xdr:row>19</xdr:row>
       <xdr:rowOff>19050</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>12</xdr:col>
       <xdr:colOff>190500</xdr:colOff>
-      <xdr:row>37</xdr:row>
+      <xdr:row>38</xdr:row>
       <xdr:rowOff>95250</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -1147,13 +1188,13 @@
     <xdr:from>
       <xdr:col>7</xdr:col>
       <xdr:colOff>600075</xdr:colOff>
-      <xdr:row>39</xdr:row>
+      <xdr:row>40</xdr:row>
       <xdr:rowOff>19050</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>12</xdr:col>
       <xdr:colOff>133352</xdr:colOff>
-      <xdr:row>39</xdr:row>
+      <xdr:row>40</xdr:row>
       <xdr:rowOff>28575</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -1194,13 +1235,13 @@
     <xdr:from>
       <xdr:col>2</xdr:col>
       <xdr:colOff>295276</xdr:colOff>
-      <xdr:row>44</xdr:row>
+      <xdr:row>45</xdr:row>
       <xdr:rowOff>28575</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>12</xdr:col>
       <xdr:colOff>114300</xdr:colOff>
-      <xdr:row>44</xdr:row>
+      <xdr:row>45</xdr:row>
       <xdr:rowOff>38101</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -1241,13 +1282,13 @@
     <xdr:from>
       <xdr:col>11</xdr:col>
       <xdr:colOff>485775</xdr:colOff>
-      <xdr:row>21</xdr:row>
+      <xdr:row>22</xdr:row>
       <xdr:rowOff>104774</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>18</xdr:col>
       <xdr:colOff>581025</xdr:colOff>
-      <xdr:row>30</xdr:row>
+      <xdr:row>31</xdr:row>
       <xdr:rowOff>47625</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -1363,13 +1404,13 @@
     <xdr:from>
       <xdr:col>2</xdr:col>
       <xdr:colOff>438151</xdr:colOff>
-      <xdr:row>13</xdr:row>
+      <xdr:row>14</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>11</xdr:col>
       <xdr:colOff>447675</xdr:colOff>
-      <xdr:row>21</xdr:row>
+      <xdr:row>22</xdr:row>
       <xdr:rowOff>161925</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -2535,11 +2576,9 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:U64"/>
+  <dimension ref="A1:U65"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="U9" sqref="U9"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -2551,7 +2590,7 @@
   <sheetData>
     <row r="1" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
-        <v>98</v>
+        <v>128</v>
       </c>
       <c r="B1" s="3"/>
       <c r="C1" s="3"/>
@@ -2586,7 +2625,7 @@
       <c r="J2" s="3"/>
       <c r="K2" s="6"/>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
         <v>50</v>
       </c>
@@ -2601,12 +2640,12 @@
       <c r="J3" s="3"/>
       <c r="K3" s="6"/>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="5">
         <v>1</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>6</v>
+        <v>125</v>
       </c>
       <c r="C4" s="3"/>
       <c r="D4" s="3"/>
@@ -2615,8 +2654,10 @@
       <c r="G4" s="3"/>
       <c r="H4" s="3"/>
       <c r="I4" s="3"/>
-      <c r="J4" s="3"/>
-      <c r="K4" s="6"/>
+      <c r="J4" s="41" t="s">
+        <v>127</v>
+      </c>
+      <c r="K4" s="42"/>
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A5" s="5">
@@ -2670,8 +2711,8 @@
       <c r="K7" s="6"/>
     </row>
     <row r="8" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A8" s="3" t="s">
-        <v>22</v>
+      <c r="A8" s="40" t="s">
+        <v>126</v>
       </c>
       <c r="B8" s="3"/>
       <c r="C8" s="3"/>
@@ -2686,92 +2727,92 @@
     </row>
     <row r="9" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="B9" s="3"/>
+      <c r="C9" s="3"/>
+      <c r="D9" s="3"/>
+      <c r="E9" s="3"/>
+      <c r="F9" s="3"/>
+      <c r="G9" s="3"/>
+      <c r="H9" s="3"/>
+      <c r="I9" s="3"/>
+      <c r="J9" s="3"/>
+      <c r="K9" s="6"/>
+    </row>
+    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A10" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="B9" s="3" t="s">
+      <c r="B10" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="C9" s="3" t="s">
+      <c r="C10" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="D9" s="3" t="s">
+      <c r="D10" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="E9" s="3" t="s">
+      <c r="E10" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="F9" s="3" t="s">
+      <c r="F10" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="G9" s="3" t="s">
+      <c r="G10" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="H9" s="3" t="s">
+      <c r="H10" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="I9" s="3" t="s">
+      <c r="I10" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="J9" s="3" t="s">
+      <c r="J10" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="K9" s="6"/>
-    </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A10" s="1">
-        <v>0</v>
-      </c>
-      <c r="B10" s="1">
-        <v>0</v>
-      </c>
-      <c r="C10" s="1">
-        <v>0</v>
-      </c>
-      <c r="D10" s="1">
-        <v>0</v>
-      </c>
-      <c r="E10" s="1">
-        <v>0</v>
-      </c>
-      <c r="F10" s="1">
-        <v>0</v>
-      </c>
-      <c r="G10" s="1">
-        <v>0</v>
-      </c>
-      <c r="H10" s="1">
-        <v>0</v>
-      </c>
-      <c r="I10" s="1">
-        <v>0</v>
-      </c>
-      <c r="J10" s="1">
-        <v>0</v>
-      </c>
       <c r="K10" s="6"/>
     </row>
     <row r="11" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A11" s="5">
+      <c r="A11" s="1">
+        <v>0</v>
+      </c>
+      <c r="B11" s="1">
+        <v>0</v>
+      </c>
+      <c r="C11" s="1">
+        <v>0</v>
+      </c>
+      <c r="D11" s="1">
+        <v>0</v>
+      </c>
+      <c r="E11" s="1">
+        <v>0</v>
+      </c>
+      <c r="F11" s="1">
+        <v>0</v>
+      </c>
+      <c r="G11" s="1">
+        <v>0</v>
+      </c>
+      <c r="H11" s="1">
+        <v>0</v>
+      </c>
+      <c r="I11" s="1">
+        <v>0</v>
+      </c>
+      <c r="J11" s="1">
+        <v>0</v>
+      </c>
+      <c r="K11" s="6"/>
+    </row>
+    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A12" s="5">
         <v>1</v>
       </c>
-      <c r="B11" s="3" t="s">
+      <c r="B12" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="C11" s="3"/>
-      <c r="D11" s="3"/>
-      <c r="E11" s="3"/>
-      <c r="F11" s="3"/>
-      <c r="G11" s="3"/>
-      <c r="H11" s="3"/>
-      <c r="I11" s="3"/>
-      <c r="J11" s="3"/>
-      <c r="K11" s="6"/>
-    </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A12" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="B12" s="3"/>
       <c r="C12" s="3"/>
       <c r="D12" s="3"/>
       <c r="E12" s="3"/>
@@ -2783,12 +2824,10 @@
       <c r="K12" s="6"/>
     </row>
     <row r="13" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A13" s="1">
-        <v>1</v>
-      </c>
-      <c r="B13" s="3" t="s">
-        <v>100</v>
-      </c>
+      <c r="A13" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B13" s="3"/>
       <c r="C13" s="3"/>
       <c r="D13" s="3"/>
       <c r="E13" s="3"/>
@@ -2801,10 +2840,10 @@
     </row>
     <row r="14" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>23</v>
+        <v>100</v>
       </c>
       <c r="C14" s="3"/>
       <c r="D14" s="3"/>
@@ -2818,10 +2857,10 @@
     </row>
     <row r="15" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
-        <v>0.2</v>
+        <v>2</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C15" s="3"/>
       <c r="D15" s="3"/>
@@ -2834,10 +2873,12 @@
       <c r="K15" s="6"/>
     </row>
     <row r="16" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A16" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="B16" s="3"/>
+      <c r="A16" s="1">
+        <v>0.2</v>
+      </c>
+      <c r="B16" s="3" t="s">
+        <v>24</v>
+      </c>
       <c r="C16" s="3"/>
       <c r="D16" s="3"/>
       <c r="E16" s="3"/>
@@ -2850,23 +2891,13 @@
     </row>
     <row r="17" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="B17" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="C17" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="D17" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="E17" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="F17" s="3" t="s">
-        <v>48</v>
-      </c>
+        <v>35</v>
+      </c>
+      <c r="B17" s="3"/>
+      <c r="C17" s="3"/>
+      <c r="D17" s="3"/>
+      <c r="E17" s="3"/>
+      <c r="F17" s="3"/>
       <c r="G17" s="3"/>
       <c r="H17" s="3"/>
       <c r="I17" s="3"/>
@@ -2874,54 +2905,62 @@
       <c r="K17" s="6"/>
     </row>
     <row r="18" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A18" s="1">
+      <c r="A18" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="B18" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="C18" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="D18" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="E18" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="F18" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="G18" s="3"/>
+      <c r="H18" s="3"/>
+      <c r="I18" s="3"/>
+      <c r="J18" s="3"/>
+      <c r="K18" s="6"/>
+    </row>
+    <row r="19" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A19" s="1">
         <v>-999</v>
       </c>
-      <c r="B18" s="1">
-        <v>0</v>
-      </c>
-      <c r="C18" s="1">
+      <c r="B19" s="1">
+        <v>0</v>
+      </c>
+      <c r="C19" s="1">
         <v>-10</v>
       </c>
-      <c r="D18" s="1">
-        <v>0</v>
-      </c>
-      <c r="E18" s="1">
+      <c r="D19" s="1">
+        <v>0</v>
+      </c>
+      <c r="E19" s="1">
         <v>1989</v>
       </c>
-      <c r="F18" s="1">
+      <c r="F19" s="1">
         <v>2016</v>
       </c>
-      <c r="G18" s="11" t="s">
+      <c r="G19" s="11" t="s">
         <v>111</v>
       </c>
-      <c r="H18" s="12"/>
-      <c r="I18" s="12"/>
-      <c r="J18" s="13"/>
-      <c r="K18" s="6"/>
-    </row>
-    <row r="19" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A19" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="B19" s="3"/>
-      <c r="C19" s="3"/>
-      <c r="D19" s="3"/>
-      <c r="E19" s="3"/>
-      <c r="F19" s="3"/>
-      <c r="G19" s="3"/>
-      <c r="H19" s="3"/>
-      <c r="I19" s="3"/>
-      <c r="J19" s="3"/>
+      <c r="H19" s="12"/>
+      <c r="I19" s="12"/>
+      <c r="J19" s="13"/>
       <c r="K19" s="6"/>
     </row>
     <row r="20" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A20" s="1">
-        <v>1</v>
-      </c>
-      <c r="B20" s="3" t="s">
-        <v>83</v>
-      </c>
+      <c r="A20" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B20" s="3"/>
       <c r="C20" s="3"/>
       <c r="D20" s="3"/>
       <c r="E20" s="3"/>
@@ -2937,7 +2976,7 @@
         <v>1</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>109</v>
+        <v>83</v>
       </c>
       <c r="C21" s="3"/>
       <c r="D21" s="3"/>
@@ -2948,25 +2987,13 @@
       <c r="I21" s="3"/>
       <c r="J21" s="3"/>
       <c r="K21" s="6"/>
-      <c r="L21" s="8" t="s">
-        <v>110</v>
-      </c>
-      <c r="M21" s="9"/>
-      <c r="N21" s="9"/>
-      <c r="O21" s="9"/>
-      <c r="P21" s="9"/>
-      <c r="Q21" s="9"/>
-      <c r="R21" s="9"/>
-      <c r="S21" s="9"/>
-      <c r="T21" s="9"/>
-      <c r="U21" s="10"/>
     </row>
     <row r="22" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A22" s="3" t="s">
-        <v>0</v>
+      <c r="A22" s="1">
+        <v>1</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>84</v>
+        <v>109</v>
       </c>
       <c r="C22" s="3"/>
       <c r="D22" s="3"/>
@@ -2977,13 +3004,25 @@
       <c r="I22" s="3"/>
       <c r="J22" s="3"/>
       <c r="K22" s="6"/>
+      <c r="L22" s="8" t="s">
+        <v>110</v>
+      </c>
+      <c r="M22" s="9"/>
+      <c r="N22" s="9"/>
+      <c r="O22" s="9"/>
+      <c r="P22" s="9"/>
+      <c r="Q22" s="9"/>
+      <c r="R22" s="9"/>
+      <c r="S22" s="9"/>
+      <c r="T22" s="9"/>
+      <c r="U22" s="10"/>
     </row>
     <row r="23" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A23" s="1">
-        <v>0.4</v>
+      <c r="A23" s="3" t="s">
+        <v>0</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>25</v>
+        <v>84</v>
       </c>
       <c r="C23" s="3"/>
       <c r="D23" s="3"/>
@@ -2997,10 +3036,10 @@
     </row>
     <row r="24" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A24" s="1">
-        <v>0.1</v>
+        <v>0.4</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C24" s="3"/>
       <c r="D24" s="3"/>
@@ -3014,10 +3053,10 @@
     </row>
     <row r="25" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A25" s="1">
-        <v>0.75</v>
+        <v>0.1</v>
       </c>
       <c r="B25" s="3" t="s">
-        <v>85</v>
+        <v>26</v>
       </c>
       <c r="C25" s="3"/>
       <c r="D25" s="3"/>
@@ -3030,11 +3069,11 @@
       <c r="K25" s="6"/>
     </row>
     <row r="26" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A26" s="3" t="s">
-        <v>0</v>
+      <c r="A26" s="1">
+        <v>0.75</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C26" s="3"/>
       <c r="D26" s="3"/>
@@ -3047,11 +3086,11 @@
       <c r="K26" s="6"/>
     </row>
     <row r="27" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A27" s="1">
-        <v>3</v>
+      <c r="A27" s="3" t="s">
+        <v>0</v>
       </c>
       <c r="B27" s="3" t="s">
-        <v>27</v>
+        <v>86</v>
       </c>
       <c r="C27" s="3"/>
       <c r="D27" s="3"/>
@@ -3068,7 +3107,7 @@
         <v>3</v>
       </c>
       <c r="B28" s="3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C28" s="3"/>
       <c r="D28" s="3"/>
@@ -3082,10 +3121,10 @@
     </row>
     <row r="29" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A29" s="1">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="B29" s="3" t="s">
-        <v>87</v>
+        <v>28</v>
       </c>
       <c r="C29" s="3"/>
       <c r="D29" s="3"/>
@@ -3098,11 +3137,11 @@
       <c r="K29" s="6"/>
     </row>
     <row r="30" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A30" s="3" t="s">
-        <v>0</v>
+      <c r="A30" s="1">
+        <v>1</v>
       </c>
       <c r="B30" s="3" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C30" s="3"/>
       <c r="D30" s="3"/>
@@ -3115,11 +3154,11 @@
       <c r="K30" s="6"/>
     </row>
     <row r="31" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A31" s="1">
-        <v>1</v>
+      <c r="A31" s="3" t="s">
+        <v>0</v>
       </c>
       <c r="B31" s="3" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C31" s="3"/>
       <c r="D31" s="3"/>
@@ -3133,10 +3172,10 @@
     </row>
     <row r="32" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A32" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B32" s="3" t="s">
-        <v>29</v>
+        <v>89</v>
       </c>
       <c r="C32" s="3"/>
       <c r="D32" s="3"/>
@@ -3149,10 +3188,12 @@
       <c r="K32" s="6"/>
     </row>
     <row r="33" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A33" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="B33" s="3"/>
+      <c r="A33" s="1">
+        <v>0</v>
+      </c>
+      <c r="B33" s="3" t="s">
+        <v>29</v>
+      </c>
       <c r="C33" s="3"/>
       <c r="D33" s="3"/>
       <c r="E33" s="3"/>
@@ -3164,12 +3205,10 @@
       <c r="K33" s="6"/>
     </row>
     <row r="34" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A34" s="1">
-        <v>2010</v>
-      </c>
-      <c r="B34" s="3" t="s">
-        <v>30</v>
-      </c>
+      <c r="A34" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B34" s="3"/>
       <c r="C34" s="3"/>
       <c r="D34" s="3"/>
       <c r="E34" s="3"/>
@@ -3182,10 +3221,10 @@
     </row>
     <row r="35" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A35" s="1">
-        <v>0</v>
+        <v>2010</v>
       </c>
       <c r="B35" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C35" s="3"/>
       <c r="D35" s="3"/>
@@ -3202,7 +3241,7 @@
         <v>0</v>
       </c>
       <c r="B36" s="3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C36" s="3"/>
       <c r="D36" s="3"/>
@@ -3216,10 +3255,10 @@
     </row>
     <row r="37" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A37" s="1">
-        <v>1999</v>
+        <v>0</v>
       </c>
       <c r="B37" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C37" s="3"/>
       <c r="D37" s="3"/>
@@ -3233,10 +3272,10 @@
     </row>
     <row r="38" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A38" s="1">
-        <v>2002</v>
+        <v>1999</v>
       </c>
       <c r="B38" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C38" s="3"/>
       <c r="D38" s="3"/>
@@ -3249,10 +3288,12 @@
       <c r="K38" s="6"/>
     </row>
     <row r="39" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A39" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="B39" s="3"/>
+      <c r="A39" s="1">
+        <v>2002</v>
+      </c>
+      <c r="B39" s="3" t="s">
+        <v>34</v>
+      </c>
       <c r="C39" s="3"/>
       <c r="D39" s="3"/>
       <c r="E39" s="3"/>
@@ -3264,12 +3305,10 @@
       <c r="K39" s="6"/>
     </row>
     <row r="40" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A40" s="1">
-        <v>1</v>
-      </c>
-      <c r="B40" s="3" t="s">
-        <v>12</v>
-      </c>
+      <c r="A40" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B40" s="3"/>
       <c r="C40" s="3"/>
       <c r="D40" s="3"/>
       <c r="E40" s="3"/>
@@ -3282,10 +3321,10 @@
     </row>
     <row r="41" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A41" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B41" s="3" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C41" s="3"/>
       <c r="D41" s="3"/>
@@ -3298,10 +3337,12 @@
       <c r="K41" s="6"/>
     </row>
     <row r="42" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A42" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="B42" s="3"/>
+      <c r="A42" s="1">
+        <v>2</v>
+      </c>
+      <c r="B42" s="3" t="s">
+        <v>11</v>
+      </c>
       <c r="C42" s="3"/>
       <c r="D42" s="3"/>
       <c r="E42" s="3"/>
@@ -3314,7 +3355,7 @@
     </row>
     <row r="43" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A43" s="3" t="s">
-        <v>93</v>
+        <v>1</v>
       </c>
       <c r="B43" s="3"/>
       <c r="C43" s="3"/>
@@ -3329,11 +3370,9 @@
     </row>
     <row r="44" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A44" s="3" t="s">
-        <v>90</v>
-      </c>
-      <c r="B44" s="3" t="s">
-        <v>94</v>
-      </c>
+        <v>93</v>
+      </c>
+      <c r="B44" s="3"/>
       <c r="C44" s="3"/>
       <c r="D44" s="3"/>
       <c r="E44" s="3"/>
@@ -3346,10 +3385,10 @@
     </row>
     <row r="45" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A45" s="3" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="B45" s="3" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C45" s="3"/>
       <c r="D45" s="3"/>
@@ -3363,10 +3402,10 @@
     </row>
     <row r="46" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A46" s="3" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="B46" s="3" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C46" s="3"/>
       <c r="D46" s="3"/>
@@ -3380,9 +3419,11 @@
     </row>
     <row r="47" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A47" s="3" t="s">
-        <v>97</v>
-      </c>
-      <c r="B47" s="3"/>
+        <v>91</v>
+      </c>
+      <c r="B47" s="3" t="s">
+        <v>96</v>
+      </c>
       <c r="C47" s="3"/>
       <c r="D47" s="3"/>
       <c r="E47" s="3"/>
@@ -3394,12 +3435,10 @@
       <c r="K47" s="6"/>
     </row>
     <row r="48" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A48" s="1">
-        <v>-9999</v>
-      </c>
-      <c r="B48" s="1">
-        <v>1</v>
-      </c>
+      <c r="A48" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="B48" s="3"/>
       <c r="C48" s="3"/>
       <c r="D48" s="3"/>
       <c r="E48" s="3"/>
@@ -3411,10 +3450,12 @@
       <c r="K48" s="6"/>
     </row>
     <row r="49" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A49" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="B49" s="3"/>
+      <c r="A49" s="1">
+        <v>-9999</v>
+      </c>
+      <c r="B49" s="1">
+        <v>1</v>
+      </c>
       <c r="C49" s="3"/>
       <c r="D49" s="3"/>
       <c r="E49" s="3"/>
@@ -3426,12 +3467,10 @@
       <c r="K49" s="6"/>
     </row>
     <row r="50" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A50" s="1">
-        <v>-9999</v>
-      </c>
-      <c r="B50" s="1">
-        <v>1</v>
-      </c>
+      <c r="A50" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="B50" s="3"/>
       <c r="C50" s="3"/>
       <c r="D50" s="3"/>
       <c r="E50" s="3"/>
@@ -3443,10 +3482,12 @@
       <c r="K50" s="6"/>
     </row>
     <row r="51" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A51" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="B51" s="3"/>
+      <c r="A51" s="1">
+        <v>-9999</v>
+      </c>
+      <c r="B51" s="1">
+        <v>1</v>
+      </c>
       <c r="C51" s="3"/>
       <c r="D51" s="3"/>
       <c r="E51" s="3"/>
@@ -3458,12 +3499,10 @@
       <c r="K51" s="6"/>
     </row>
     <row r="52" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A52" s="1">
-        <v>-9999</v>
-      </c>
-      <c r="B52" s="1">
-        <v>-1</v>
-      </c>
+      <c r="A52" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="B52" s="3"/>
       <c r="C52" s="3"/>
       <c r="D52" s="3"/>
       <c r="E52" s="3"/>
@@ -3475,10 +3514,12 @@
       <c r="K52" s="6"/>
     </row>
     <row r="53" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A53" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="B53" s="3"/>
+      <c r="A53" s="1">
+        <v>-9999</v>
+      </c>
+      <c r="B53" s="1">
+        <v>-1</v>
+      </c>
       <c r="C53" s="3"/>
       <c r="D53" s="3"/>
       <c r="E53" s="3"/>
@@ -3490,12 +3531,10 @@
       <c r="K53" s="6"/>
     </row>
     <row r="54" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A54" s="1">
-        <v>-9999</v>
-      </c>
-      <c r="B54" s="1">
-        <v>-1</v>
-      </c>
+      <c r="A54" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="B54" s="3"/>
       <c r="C54" s="3"/>
       <c r="D54" s="3"/>
       <c r="E54" s="3"/>
@@ -3507,10 +3546,12 @@
       <c r="K54" s="6"/>
     </row>
     <row r="55" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A55" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="B55" s="3"/>
+      <c r="A55" s="1">
+        <v>-9999</v>
+      </c>
+      <c r="B55" s="1">
+        <v>-1</v>
+      </c>
       <c r="C55" s="3"/>
       <c r="D55" s="3"/>
       <c r="E55" s="3"/>
@@ -3523,7 +3564,7 @@
     </row>
     <row r="56" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A56" s="3" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B56" s="3"/>
       <c r="C56" s="3"/>
@@ -3538,7 +3579,7 @@
     </row>
     <row r="57" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A57" s="3" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B57" s="3"/>
       <c r="C57" s="3"/>
@@ -3553,7 +3594,7 @@
     </row>
     <row r="58" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A58" s="3" t="s">
-        <v>40</v>
+        <v>4</v>
       </c>
       <c r="B58" s="3"/>
       <c r="C58" s="3"/>
@@ -3567,12 +3608,10 @@
       <c r="K58" s="6"/>
     </row>
     <row r="59" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A59" s="1">
-        <v>2</v>
-      </c>
-      <c r="B59" s="3" t="s">
-        <v>15</v>
-      </c>
+      <c r="A59" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="B59" s="3"/>
       <c r="C59" s="3"/>
       <c r="D59" s="3"/>
       <c r="E59" s="3"/>
@@ -3584,10 +3623,12 @@
       <c r="K59" s="6"/>
     </row>
     <row r="60" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A60" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="B60" s="3"/>
+      <c r="A60" s="1">
+        <v>2</v>
+      </c>
+      <c r="B60" s="3" t="s">
+        <v>15</v>
+      </c>
       <c r="C60" s="3"/>
       <c r="D60" s="3"/>
       <c r="E60" s="3"/>
@@ -3600,17 +3641,11 @@
     </row>
     <row r="61" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A61" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="B61" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="C61" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="D61" s="3" t="s">
-        <v>42</v>
-      </c>
+        <v>5</v>
+      </c>
+      <c r="B61" s="3"/>
+      <c r="C61" s="3"/>
+      <c r="D61" s="3"/>
       <c r="E61" s="3"/>
       <c r="F61" s="3"/>
       <c r="G61" s="3"/>
@@ -3620,17 +3655,17 @@
       <c r="K61" s="6"/>
     </row>
     <row r="62" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A62" s="1">
-        <v>-9999</v>
-      </c>
-      <c r="B62" s="1">
-        <v>1</v>
-      </c>
-      <c r="C62" s="1">
-        <v>1</v>
-      </c>
-      <c r="D62" s="1">
-        <v>10</v>
+      <c r="A62" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="B62" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C62" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D62" s="3" t="s">
+        <v>42</v>
       </c>
       <c r="E62" s="3"/>
       <c r="F62" s="3"/>
@@ -3641,12 +3676,18 @@
       <c r="K62" s="6"/>
     </row>
     <row r="63" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A63" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="B63" s="3"/>
-      <c r="C63" s="3"/>
-      <c r="D63" s="3"/>
+      <c r="A63" s="1">
+        <v>-9999</v>
+      </c>
+      <c r="B63" s="1">
+        <v>1</v>
+      </c>
+      <c r="C63" s="1">
+        <v>1</v>
+      </c>
+      <c r="D63" s="1">
+        <v>10</v>
+      </c>
       <c r="E63" s="3"/>
       <c r="F63" s="3"/>
       <c r="G63" s="3"/>
@@ -3656,12 +3697,10 @@
       <c r="K63" s="6"/>
     </row>
     <row r="64" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A64" s="1">
-        <v>999</v>
-      </c>
-      <c r="B64" s="3" t="s">
-        <v>82</v>
-      </c>
+      <c r="A64" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B64" s="3"/>
       <c r="C64" s="3"/>
       <c r="D64" s="3"/>
       <c r="E64" s="3"/>
@@ -3671,6 +3710,23 @@
       <c r="I64" s="3"/>
       <c r="J64" s="3"/>
       <c r="K64" s="6"/>
+    </row>
+    <row r="65" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A65" s="1">
+        <v>999</v>
+      </c>
+      <c r="B65" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="C65" s="3"/>
+      <c r="D65" s="3"/>
+      <c r="E65" s="3"/>
+      <c r="F65" s="3"/>
+      <c r="G65" s="3"/>
+      <c r="H65" s="3"/>
+      <c r="I65" s="3"/>
+      <c r="J65" s="3"/>
+      <c r="K65" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -5981,7 +6037,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q64"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A7" workbookViewId="0">
       <selection activeCell="U27" sqref="U27"/>
     </sheetView>
   </sheetViews>

</xml_diff>